<commit_message>
fix result grading in templates
</commit_message>
<xml_diff>
--- a/static/excel/templates/spreadsheet_template.xlsx
+++ b/static/excel/templates/spreadsheet_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F73692F6-EC8C-4BDE-9349-6829E070F648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF9F0F-FB5E-4257-B18F-8EAC0FA2193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" tabRatio="741" xr2:uid="{0136EA61-87B7-4DCD-8EF4-D0D6798CF37A}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="741" xr2:uid="{0136EA61-87B7-4DCD-8EF4-D0D6798CF37A}"/>
   </bookViews>
   <sheets>
     <sheet name="L100" sheetId="2" r:id="rId1"/>
@@ -619,139 +619,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -765,6 +632,24 @@
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -816,6 +701,103 @@
       <protection locked="1" hidden="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -827,6 +809,24 @@
         <scheme val="none"/>
       </font>
       <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -5436,15 +5436,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{4DE29814-387D-4E88-AB23-8407891F81F2}" name="Flagged" displayName="Flagged" ref="A10:G12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{944EB04F-1BD9-42F7-8770-84EFBDC079AD}" name="Course Code" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{C26D477F-198A-4820-BEF5-C85FB09034C9}" name="Course Title" dataDxfId="18" totalsRowDxfId="11"/>
-    <tableColumn id="3" xr3:uid="{128D06A2-BCDA-4F9E-BA7B-4220D5374792}" name="CU" totalsRowFunction="sum" totalsRowDxfId="10" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{6ADFF330-D98B-45E2-8412-66E7D0DDD828}" name="Mark" totalsRowDxfId="9" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{C1C184AC-DD32-47D9-A7FE-1D08956BA12A}" name="Grade" totalsRowDxfId="8" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{944EB04F-1BD9-42F7-8770-84EFBDC079AD}" name="Course Code" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="2" xr3:uid="{C26D477F-198A-4820-BEF5-C85FB09034C9}" name="Course Title" dataDxfId="17" totalsRowDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{128D06A2-BCDA-4F9E-BA7B-4220D5374792}" name="CU" totalsRowFunction="sum" totalsRowDxfId="15" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{6ADFF330-D98B-45E2-8412-66E7D0DDD828}" name="Mark" totalsRowDxfId="14" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{C1C184AC-DD32-47D9-A7FE-1D08956BA12A}" name="Grade" totalsRowDxfId="13" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(Flagged[[#This Row],[Mark]]="","",IF(AND(LEN(Flagged[[#This Row],[Course Code]])=10, Flagged[[#This Row],[Mark]]&gt;=60),"C",IF(Flagged[[#This Row],[Mark]]&lt;40,"F",IF(Flagged[[#This Row],[Mark]]&lt;45,"E",IF(Flagged[[#This Row],[Mark]]&lt;50,"D",IF(Flagged[[#This Row],[Mark]]&lt;60,"C",IF(Flagged[[#This Row],[Mark]]&lt;70,"B",IF(Flagged[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C792FA37-5431-40E6-B8D7-5AF59CBE55D7}" name="Session" totalsRowDxfId="7" dataCellStyle="Number Style"/>
-    <tableColumn id="7" xr3:uid="{C62DA4E8-E108-42E6-A0AA-53F1BCCF6CD9}" name="Reason" totalsRowDxfId="6" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{C792FA37-5431-40E6-B8D7-5AF59CBE55D7}" name="Session" totalsRowDxfId="12" dataCellStyle="Number Style"/>
+    <tableColumn id="7" xr3:uid="{C62DA4E8-E108-42E6-A0AA-53F1BCCF6CD9}" name="Reason" totalsRowDxfId="11" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5473,11 +5473,11 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{04B5BFC3-8AA9-427D-8CF3-80475AFDC6F5}" name="Unknown" displayName="Unknown" ref="A10:F12" totalsRowCount="1" headerRowDxfId="17" dataDxfId="16" totalsRowDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{04B5BFC3-8AA9-427D-8CF3-80475AFDC6F5}" name="Unknown" displayName="Unknown" ref="A10:F12" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
   <autoFilter ref="A10:F11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{76D571A1-3DFE-47CD-9113-AD850BC06622}" name="Course Code" totalsRowLabel="Total" dataDxfId="14" totalsRowDxfId="5"/>
-    <tableColumn id="2" xr3:uid="{C6F77A54-E001-4630-A19B-A21D9D2F0F20}" name="Course Title" dataDxfId="13" totalsRowDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{76D571A1-3DFE-47CD-9113-AD850BC06622}" name="Course Code" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C6F77A54-E001-4630-A19B-A21D9D2F0F20}" name="Course Title" dataDxfId="5" totalsRowDxfId="4"/>
     <tableColumn id="3" xr3:uid="{1998C348-2D03-4F42-80A1-BC05E3A48BC1}" name="CU" totalsRowFunction="sum" totalsRowDxfId="3" dataCellStyle="Number Style"/>
     <tableColumn id="4" xr3:uid="{3FD1F606-8400-4AB0-8EF7-490910A85DF9}" name="Mark" totalsRowDxfId="2" dataCellStyle="Number Style"/>
     <tableColumn id="5" xr3:uid="{AFFE1CA0-63C6-4DB6-AC76-A3C8D5D4C4D0}" name="Grade" totalsRowDxfId="1" dataCellStyle="Number Style">
@@ -5949,15 +5949,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="8" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="8" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="8" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="63" t="s">
         <v>21</v>
       </c>
@@ -5968,7 +5968,7 @@
       <c r="F1" s="63"/>
       <c r="G1" s="63"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="64" t="s">
         <v>39</v>
       </c>
@@ -5979,7 +5979,7 @@
       <c r="F2" s="64"/>
       <c r="G2" s="64"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="64" t="s">
         <v>40</v>
       </c>
@@ -5990,7 +5990,7 @@
       <c r="F3" s="64"/>
       <c r="G3" s="64"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="61" t="s">
         <v>20</v>
       </c>
@@ -6001,7 +6001,7 @@
       <c r="F4" s="61"/>
       <c r="G4" s="61"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="9"/>
@@ -6010,7 +6010,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="9"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="43" t="s">
         <v>19</v>
       </c>
@@ -6023,7 +6023,7 @@
       <c r="F6" s="65"/>
       <c r="G6" s="66"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="44" t="s">
         <v>17</v>
       </c>
@@ -6038,7 +6038,7 @@
       </c>
       <c r="G7" s="14"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="61" t="s">
         <v>14</v>
       </c>
@@ -6049,7 +6049,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -6072,7 +6072,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -6090,7 +6090,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -6106,7 +6106,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="36" t="s">
         <v>13</v>
       </c>
@@ -6120,7 +6120,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="8" t="s">
         <v>12</v>
       </c>
@@ -6143,7 +6143,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -6161,7 +6161,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="8" t="s">
         <v>5</v>
       </c>
@@ -6177,7 +6177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C19" s="16" t="s">
         <v>4</v>
       </c>
@@ -6193,7 +6193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -6212,13 +6212,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -6257,17 +6257,17 @@
       <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.20703125" style="8" customWidth="1"/>
-    <col min="3" max="5" width="7.5390625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="8" customWidth="1"/>
-    <col min="7" max="7" width="102.95703125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="33.1875" style="8" customWidth="1"/>
+    <col min="3" max="5" width="7.5234375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.80859375" style="8" customWidth="1"/>
+    <col min="7" max="7" width="102.94921875" style="8" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -6278,7 +6278,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="58"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -6290,7 +6290,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="58"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -6302,7 +6302,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="58"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="63" t="s">
         <v>43</v>
       </c>
@@ -6313,7 +6313,7 @@
       <c r="F6" s="63"/>
       <c r="G6" s="58"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -6321,7 +6321,7 @@
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -6329,7 +6329,7 @@
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="54"/>
       <c r="B9" s="54"/>
       <c r="C9" s="55"/>
@@ -6337,7 +6337,7 @@
       <c r="E9" s="55"/>
       <c r="F9" s="55"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -6360,7 +6360,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -6372,7 +6372,7 @@
       <c r="F11" s="38"/>
       <c r="G11"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -6385,7 +6385,7 @@
       <c r="F12" s="34"/>
       <c r="G12" s="59"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -6393,7 +6393,7 @@
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -6401,7 +6401,7 @@
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -6409,7 +6409,7 @@
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -6417,7 +6417,7 @@
       <c r="E17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -6425,7 +6425,7 @@
       <c r="E18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -6433,7 +6433,7 @@
       <c r="E19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -6441,7 +6441,7 @@
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -6449,7 +6449,7 @@
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -6457,7 +6457,7 @@
       <c r="E22"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -6465,7 +6465,7 @@
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -6473,7 +6473,7 @@
       <c r="E24"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -6481,7 +6481,7 @@
       <c r="E25"/>
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -6517,16 +6517,16 @@
       <selection activeCell="A6" sqref="A6:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.20703125" style="8" customWidth="1"/>
-    <col min="3" max="5" width="7.5390625" style="8" customWidth="1"/>
-    <col min="6" max="6" width="13.83203125" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="33.1875" style="8" customWidth="1"/>
+    <col min="3" max="5" width="7.5234375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.80859375" style="8" customWidth="1"/>
     <col min="7" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -6537,7 +6537,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="53"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -6549,7 +6549,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="53"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -6561,7 +6561,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="53"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="63" t="s">
         <v>41</v>
       </c>
@@ -6571,7 +6571,7 @@
       <c r="E6" s="63"/>
       <c r="F6" s="63"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7"/>
       <c r="B7"/>
       <c r="C7"/>
@@ -6579,7 +6579,7 @@
       <c r="E7"/>
       <c r="F7"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A8"/>
       <c r="B8"/>
       <c r="C8"/>
@@ -6587,7 +6587,7 @@
       <c r="E8"/>
       <c r="F8"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="51"/>
       <c r="B9" s="51"/>
       <c r="C9" s="52"/>
@@ -6595,7 +6595,7 @@
       <c r="E9" s="52"/>
       <c r="F9" s="52"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
@@ -6615,7 +6615,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -6626,7 +6626,7 @@
       </c>
       <c r="F11" s="38"/>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="8" t="s">
         <v>5</v>
       </c>
@@ -6638,7 +6638,7 @@
       <c r="E12" s="34"/>
       <c r="F12" s="34"/>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A14"/>
       <c r="B14"/>
       <c r="C14"/>
@@ -6646,7 +6646,7 @@
       <c r="E14"/>
       <c r="F14"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15"/>
       <c r="B15"/>
       <c r="C15"/>
@@ -6654,7 +6654,7 @@
       <c r="E15"/>
       <c r="F15"/>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16"/>
       <c r="B16"/>
       <c r="C16"/>
@@ -6662,7 +6662,7 @@
       <c r="E16"/>
       <c r="F16"/>
     </row>
-    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17"/>
       <c r="B17"/>
       <c r="C17"/>
@@ -6670,7 +6670,7 @@
       <c r="E17"/>
       <c r="F17"/>
     </row>
-    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18"/>
       <c r="B18"/>
       <c r="C18"/>
@@ -6678,7 +6678,7 @@
       <c r="E18"/>
       <c r="F18"/>
     </row>
-    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A19"/>
       <c r="B19"/>
       <c r="C19"/>
@@ -6686,7 +6686,7 @@
       <c r="E19"/>
       <c r="F19"/>
     </row>
-    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -6694,7 +6694,7 @@
       <c r="E20"/>
       <c r="F20"/>
     </row>
-    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21"/>
@@ -6702,7 +6702,7 @@
       <c r="E21"/>
       <c r="F21"/>
     </row>
-    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A22"/>
       <c r="B22"/>
       <c r="C22"/>
@@ -6710,7 +6710,7 @@
       <c r="E22"/>
       <c r="F22"/>
     </row>
-    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A23"/>
       <c r="B23"/>
       <c r="C23"/>
@@ -6718,7 +6718,7 @@
       <c r="E23"/>
       <c r="F23"/>
     </row>
-    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A24"/>
       <c r="B24"/>
       <c r="C24"/>
@@ -6726,7 +6726,7 @@
       <c r="E24"/>
       <c r="F24"/>
     </row>
-    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A25"/>
       <c r="B25"/>
       <c r="C25"/>
@@ -6734,7 +6734,7 @@
       <c r="E25"/>
       <c r="F25"/>
     </row>
-    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A26"/>
       <c r="B26"/>
       <c r="C26"/>
@@ -6770,15 +6770,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -6789,7 +6789,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -6801,7 +6801,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -6813,7 +6813,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -6824,7 +6824,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -6833,7 +6833,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -6852,7 +6852,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -6876,7 +6876,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>22</v>
       </c>
@@ -6887,7 +6887,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -6910,7 +6910,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -6928,7 +6928,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -6944,7 +6944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>23</v>
       </c>
@@ -6958,7 +6958,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -6981,7 +6981,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -6999,7 +6999,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -7015,7 +7015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
@@ -7031,7 +7031,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -7050,13 +7050,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -7098,15 +7098,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -7117,7 +7117,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -7129,7 +7129,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -7141,7 +7141,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -7152,7 +7152,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -7161,7 +7161,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -7180,7 +7180,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -7204,7 +7204,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>24</v>
       </c>
@@ -7215,7 +7215,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -7238,7 +7238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -7256,7 +7256,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -7272,7 +7272,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>25</v>
       </c>
@@ -7286,7 +7286,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -7309,7 +7309,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -7327,7 +7327,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -7343,7 +7343,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C19" s="25" t="s">
         <v>4</v>
       </c>
@@ -7359,7 +7359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -7378,13 +7378,13 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -7426,15 +7426,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -7445,7 +7445,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -7457,7 +7457,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -7469,7 +7469,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -7480,7 +7480,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -7489,7 +7489,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -7508,7 +7508,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -7532,7 +7532,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>26</v>
       </c>
@@ -7543,7 +7543,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -7566,7 +7566,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -7584,7 +7584,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -7600,7 +7600,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>27</v>
       </c>
@@ -7614,7 +7614,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -7637,7 +7637,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -7655,7 +7655,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -7671,12 +7671,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="56"/>
       <c r="G18" s="56"/>
       <c r="H18"/>
     </row>
-    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="56"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
@@ -7694,7 +7694,7 @@
       </c>
       <c r="H19"/>
     </row>
-    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -7714,7 +7714,7 @@
       </c>
       <c r="H20"/>
     </row>
-    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
@@ -7722,7 +7722,7 @@
       <c r="G21" s="56"/>
       <c r="H21"/>
     </row>
-    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -7736,14 +7736,14 @@
       <c r="F22"/>
       <c r="G22"/>
     </row>
-    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C23"/>
       <c r="D23"/>
       <c r="E23"/>
       <c r="F23"/>
       <c r="G23"/>
     </row>
-    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="C24"/>
       <c r="D24"/>
       <c r="E24"/>
@@ -7783,16 +7783,16 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="3" width="7.5390625" style="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="3" width="7.5234375" style="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -7803,7 +7803,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -7815,7 +7815,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -7827,7 +7827,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -7838,7 +7838,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -7847,7 +7847,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -7866,7 +7866,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -7890,7 +7890,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>28</v>
       </c>
@@ -7901,7 +7901,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -7924,7 +7924,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -7942,7 +7942,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -7958,7 +7958,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>29</v>
       </c>
@@ -7972,7 +7972,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -7995,7 +7995,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -8013,7 +8013,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -8029,11 +8029,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="42"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
@@ -8050,7 +8050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -8069,14 +8069,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
       <c r="G21" s="29"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -8095,7 +8095,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -8108,7 +8108,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="7" t="str">
-        <f>IF(G20&gt;4.49,"1",IF(G20&gt;3.49,"2.1",IF(G20&gt;2.39,"2.2",IF(G20&gt;1.49,"3rd","Pass"))))</f>
+        <f>IF(G20&gt;=4.495,"1",IF(G20&gt;=3.495,"2.1",IF(G20&gt;=2.395,"2.2",IF(G20&gt;=1.495,"3rd","Pass"))))</f>
         <v>Pass</v>
       </c>
     </row>
@@ -8145,15 +8145,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -8164,7 +8164,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -8176,7 +8176,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -8188,7 +8188,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -8199,7 +8199,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -8208,7 +8208,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -8227,7 +8227,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -8251,7 +8251,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>30</v>
       </c>
@@ -8262,7 +8262,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -8285,7 +8285,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -8303,7 +8303,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -8319,7 +8319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>31</v>
       </c>
@@ -8333,7 +8333,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -8356,7 +8356,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -8374,7 +8374,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -8390,11 +8390,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="28"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
@@ -8411,7 +8411,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -8431,14 +8431,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
       <c r="G21" s="29"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -8457,7 +8457,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -8470,7 +8470,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="7" t="str">
-        <f>IF(G20&gt;4.49,"1",IF(G20&gt;3.49,"2.1",IF(G20&gt;2.39,"2.2",IF(G20&gt;1.49,"3rd","Pass"))))</f>
+        <f>IF(G20&gt;=4.495,"1",IF(G20&gt;=3.495,"2.1",IF(G20&gt;=2.395,"2.2",IF(G20&gt;=1.495,"3rd","Pass"))))</f>
         <v>Pass</v>
       </c>
     </row>
@@ -8507,15 +8507,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -8526,7 +8526,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -8538,7 +8538,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -8550,7 +8550,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -8561,7 +8561,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
       <c r="B5" s="21"/>
       <c r="C5" s="21"/>
@@ -8570,7 +8570,7 @@
       <c r="F5" s="21"/>
       <c r="G5" s="21"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -8589,7 +8589,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -8613,7 +8613,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>32</v>
       </c>
@@ -8624,7 +8624,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -8647,7 +8647,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -8665,7 +8665,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -8681,7 +8681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>33</v>
       </c>
@@ -8695,7 +8695,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -8718,7 +8718,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -8736,7 +8736,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -8752,11 +8752,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="28"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
@@ -8773,7 +8773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -8793,14 +8793,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
       <c r="G21" s="29"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -8819,7 +8819,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -8832,7 +8832,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="7" t="str">
-        <f>IF(G20&gt;4.49,"1",IF(G20&gt;3.49,"2.1",IF(G20&gt;2.39,"2.2",IF(G20&gt;1.49,"3rd","Pass"))))</f>
+        <f>IF(G20&gt;=4.495,"1",IF(G20&gt;=3.495,"2.1",IF(G20&gt;=2.395,"2.2",IF(G20&gt;=1.495,"3rd","Pass"))))</f>
         <v>Pass</v>
       </c>
     </row>
@@ -8869,15 +8869,15 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -8888,7 +8888,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -8900,7 +8900,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -8912,7 +8912,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -8923,7 +8923,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="48"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
@@ -8932,7 +8932,7 @@
       <c r="F5" s="48"/>
       <c r="G5" s="48"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -8951,7 +8951,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -8975,7 +8975,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>32</v>
       </c>
@@ -8986,7 +8986,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -9009,7 +9009,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -9027,7 +9027,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -9043,7 +9043,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>33</v>
       </c>
@@ -9057,7 +9057,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -9080,7 +9080,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -9098,7 +9098,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -9114,11 +9114,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="28"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
@@ -9135,7 +9135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -9155,14 +9155,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
       <c r="G21" s="29"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -9181,7 +9181,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="7" t="str">
-        <f>IF(G20&gt;4.49,"1",IF(G20&gt;3.49,"2.1",IF(G20&gt;2.39,"2.2",IF(G20&gt;1.49,"3rd","Pass"))))</f>
+        <f>IF(G20&gt;=4.495,"1",IF(G20&gt;=3.495,"2.1",IF(G20&gt;=2.395,"2.2",IF(G20&gt;=1.495,"3rd","Pass"))))</f>
         <v>Pass</v>
       </c>
     </row>
@@ -9228,18 +9228,18 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection sqref="A1:G3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.65"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="13.625" style="20" customWidth="1"/>
-    <col min="2" max="2" width="43.75" style="20" customWidth="1"/>
-    <col min="3" max="7" width="7.5390625" style="20" customWidth="1"/>
+    <col min="1" max="1" width="13.6171875" style="20" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="20" customWidth="1"/>
+    <col min="3" max="7" width="7.5234375" style="20" customWidth="1"/>
     <col min="8" max="16384" width="8.6640625" style="20"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
@@ -9250,7 +9250,7 @@
       <c r="F1" s="68"/>
       <c r="G1" s="68"/>
     </row>
-    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="68" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
@@ -9262,7 +9262,7 @@
       <c r="F2" s="68"/>
       <c r="G2" s="68"/>
     </row>
-    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A3" s="68" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
@@ -9274,7 +9274,7 @@
       <c r="F3" s="68"/>
       <c r="G3" s="68"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A4" s="67" t="s">
         <v>20</v>
       </c>
@@ -9285,7 +9285,7 @@
       <c r="F4" s="67"/>
       <c r="G4" s="67"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="48"/>
       <c r="B5" s="48"/>
       <c r="C5" s="48"/>
@@ -9294,7 +9294,7 @@
       <c r="F5" s="48"/>
       <c r="G5" s="48"/>
     </row>
-    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="39" t="s">
         <v>19</v>
       </c>
@@ -9313,7 +9313,7 @@
       <c r="F6" s="69"/>
       <c r="G6" s="70"/>
     </row>
-    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
         <v>17</v>
       </c>
@@ -9337,7 +9337,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A9" s="67" t="s">
         <v>32</v>
       </c>
@@ -9348,7 +9348,7 @@
       <c r="F9" s="62"/>
       <c r="G9" s="62"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
         <v>12</v>
       </c>
@@ -9371,7 +9371,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="15"/>
       <c r="B11" s="15"/>
       <c r="C11" s="38"/>
@@ -9389,7 +9389,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A12" s="20" t="s">
         <v>5</v>
       </c>
@@ -9405,7 +9405,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A14" s="37" t="s">
         <v>33</v>
       </c>
@@ -9419,7 +9419,7 @@
       <c r="F14" s="36"/>
       <c r="G14" s="36"/>
     </row>
-    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A15" s="20" t="s">
         <v>12</v>
       </c>
@@ -9442,7 +9442,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A16" s="15"/>
       <c r="B16" s="15"/>
       <c r="C16" s="38"/>
@@ -9460,7 +9460,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="17" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A17" s="20" t="s">
         <v>5</v>
       </c>
@@ -9476,11 +9476,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="18" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A18" s="28"/>
       <c r="G18" s="29"/>
     </row>
-    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="19" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A19" s="28"/>
       <c r="C19" s="25" t="s">
         <v>4</v>
@@ -9497,7 +9497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="20" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A20" s="30" t="s">
         <v>2</v>
       </c>
@@ -9517,14 +9517,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A21" s="41" t="s">
         <v>38</v>
       </c>
       <c r="B21" s="18"/>
       <c r="G21" s="29"/>
     </row>
-    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="22" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A22" s="41" t="s">
         <v>37</v>
       </c>
@@ -9543,7 +9543,7 @@
       <c r="F22" s="2"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.7">
+    <row r="23" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="C23" s="4" t="s">
         <v>35</v>
       </c>
@@ -9556,7 +9556,7 @@
         <v>36</v>
       </c>
       <c r="G23" s="7" t="str">
-        <f>IF(G20&gt;4.49,"1",IF(G20&gt;3.49,"2.1",IF(G20&gt;2.39,"2.2",IF(G20&gt;1.49,"3rd","Pass"))))</f>
+        <f>IF(G20&gt;=4.495,"1",IF(G20&gt;=3.495,"2.1",IF(G20&gt;=2.395,"2.2",IF(G20&gt;=1.495,"3rd","Pass"))))</f>
         <v>Pass</v>
       </c>
     </row>

</xml_diff>

<commit_message>
feat: implement outstanding courses on spreadsheet
</commit_message>
<xml_diff>
--- a/static/excel/templates/spreadsheet_template.xlsx
+++ b/static/excel/templates/spreadsheet_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GOODHOPE ORDU\Documents\excel_converter\static\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AF9F0F-FB5E-4257-B18F-8EAC0FA2193F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5362179-57F8-4D6F-92A2-AE02AE9DB44F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" tabRatio="741" xr2:uid="{0136EA61-87B7-4DCD-8EF4-D0D6798CF37A}"/>
   </bookViews>
@@ -24,6 +24,7 @@
     <sheet name="L900" sheetId="10" r:id="rId9"/>
     <sheet name="Flagged Results" sheetId="12" r:id="rId10"/>
     <sheet name="Unknown Courses" sheetId="11" r:id="rId11"/>
+    <sheet name="Outstanding Courses" sheetId="13" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="46">
   <si>
     <t>CGPA =</t>
   </si>
@@ -177,6 +178,9 @@
   </si>
   <si>
     <t>Reason</t>
+  </si>
+  <si>
+    <t>OUTSTANDING COURSES</t>
   </si>
 </sst>
 </file>
@@ -372,7 +376,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
@@ -492,6 +496,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
@@ -522,7 +530,184 @@
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
     <cellStyle name="Number Style" xfId="1" xr:uid="{AC7B9499-A25A-4749-8777-7B6BAB93D474}"/>
   </cellStyles>
-  <dxfs count="242">
+  <dxfs count="253">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <protection locked="1" hidden="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -4591,9 +4776,9 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Semester Style" pivot="0" count="3" xr9:uid="{9907FA53-AAFE-4AC5-9E70-86FBD65D07FE}">
-      <tableStyleElement type="wholeTable" dxfId="241"/>
-      <tableStyleElement type="headerRow" dxfId="240"/>
-      <tableStyleElement type="totalRow" dxfId="239"/>
+      <tableStyleElement type="wholeTable" dxfId="252"/>
+      <tableStyleElement type="headerRow" dxfId="251"/>
+      <tableStyleElement type="totalRow" dxfId="250"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -4738,6 +4923,61 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D3D352A-FECC-4C23-B961-C393867255BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="547794" cy="525897"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing12.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="absolute">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>547794</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>144897</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E5A7E33C-6071-4F0A-9474-829E549EC7A3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5213,20 +5453,20 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C752E597-B7FA-401C-B3E8-88E9F8623BEB}" name="S1.1" displayName="S1.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="238" dataDxfId="237" totalsRowDxfId="236">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C752E597-B7FA-401C-B3E8-88E9F8623BEB}" name="S1.1" displayName="S1.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="249" dataDxfId="248" totalsRowDxfId="247">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{143D1874-E52E-4649-B541-CB4F2B281B22}" name="Course Code" totalsRowLabel="Total" dataDxfId="235" totalsRowDxfId="234"/>
-    <tableColumn id="2" xr3:uid="{A2FA1733-F761-4324-B70B-50DD52530A1A}" name="Course Title" dataDxfId="233" totalsRowDxfId="232"/>
-    <tableColumn id="3" xr3:uid="{B486B7EC-352A-40BD-92C7-9BAE4885CF6F}" name="CU" totalsRowFunction="sum" totalsRowDxfId="231" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{B6E798FB-74B4-4175-B14E-5AD591D12EF1}" name="Mark" totalsRowDxfId="230" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{868E38A9-6782-44F8-96E9-6FEF842D2BC9}" name="Grade" totalsRowDxfId="229" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{143D1874-E52E-4649-B541-CB4F2B281B22}" name="Course Code" totalsRowLabel="Total" dataDxfId="246" totalsRowDxfId="245"/>
+    <tableColumn id="2" xr3:uid="{A2FA1733-F761-4324-B70B-50DD52530A1A}" name="Course Title" dataDxfId="244" totalsRowDxfId="243"/>
+    <tableColumn id="3" xr3:uid="{B486B7EC-352A-40BD-92C7-9BAE4885CF6F}" name="CU" totalsRowFunction="sum" totalsRowDxfId="242" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{B6E798FB-74B4-4175-B14E-5AD591D12EF1}" name="Mark" totalsRowDxfId="241" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{868E38A9-6782-44F8-96E9-6FEF842D2BC9}" name="Grade" totalsRowDxfId="240" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S1.1[[#This Row],[Mark]]="","",IF(AND(LEN(S1.1[[#This Row],[Course Code]])=10, S1.1[[#This Row],[Mark]]&gt;=60),"C",IF(S1.1[[#This Row],[Mark]]&lt;40,"F",IF(S1.1[[#This Row],[Mark]]&lt;45,"E",IF(S1.1[[#This Row],[Mark]]&lt;50,"D",IF(S1.1[[#This Row],[Mark]]&lt;60,"C",IF(S1.1[[#This Row],[Mark]]&lt;70,"B",IF(S1.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{ACE6B92C-E74C-4411-A250-042758A737B9}" name="GP" totalsRowDxfId="228" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{ACE6B92C-E74C-4411-A250-042758A737B9}" name="GP" totalsRowDxfId="239" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S1.1[[#This Row],[Mark]]="","",IF(AND(LEN(S1.1[[#This Row],[Course Code]])=10, S1.1[[#This Row],[Mark]]&gt;=60),3,IF(S1.1[[#This Row],[Mark]]&lt;40,0,IF(S1.1[[#This Row],[Mark]]&lt;45,1,IF(S1.1[[#This Row],[Mark]]&lt;50,2,IF(S1.1[[#This Row],[Mark]]&lt;60,3,IF(S1.1[[#This Row],[Mark]]&lt;70,4,IF(S1.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F41947E5-B7CE-4B71-BA6B-157F5B092120}" name="QP" totalsRowFunction="sum" totalsRowDxfId="227" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{F41947E5-B7CE-4B71-BA6B-157F5B092120}" name="QP" totalsRowFunction="sum" totalsRowDxfId="238" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S1.1[[#This Row],[CU]]*S1.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5235,20 +5475,20 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5C102414-FC32-47BF-9CF9-79C867F18AF2}" name="S5.2" displayName="S5.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="130" dataDxfId="129" totalsRowDxfId="128">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{5C102414-FC32-47BF-9CF9-79C867F18AF2}" name="S5.2" displayName="S5.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="141" dataDxfId="140" totalsRowDxfId="139">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{318A193E-8D74-4250-A998-AE37C323E40D}" name="Course Code" totalsRowLabel="Total" dataDxfId="127" totalsRowDxfId="126"/>
-    <tableColumn id="2" xr3:uid="{B4148092-6C9F-429A-9ADC-8479BA0E4E13}" name="Course Title" dataDxfId="125" totalsRowDxfId="124"/>
-    <tableColumn id="3" xr3:uid="{5A86F6F5-207C-45A2-8547-9C24881743D2}" name="CU" totalsRowFunction="sum" totalsRowDxfId="123" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{43984D7B-69DD-43C6-BC69-1111BDC2AE8F}" name="Mark" totalsRowDxfId="122" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{19BE16CC-06D0-462A-ADDF-6066D7A3294F}" name="Grade" totalsRowDxfId="121" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{318A193E-8D74-4250-A998-AE37C323E40D}" name="Course Code" totalsRowLabel="Total" dataDxfId="138" totalsRowDxfId="137"/>
+    <tableColumn id="2" xr3:uid="{B4148092-6C9F-429A-9ADC-8479BA0E4E13}" name="Course Title" dataDxfId="136" totalsRowDxfId="135"/>
+    <tableColumn id="3" xr3:uid="{5A86F6F5-207C-45A2-8547-9C24881743D2}" name="CU" totalsRowFunction="sum" totalsRowDxfId="134" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{43984D7B-69DD-43C6-BC69-1111BDC2AE8F}" name="Mark" totalsRowDxfId="133" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{19BE16CC-06D0-462A-ADDF-6066D7A3294F}" name="Grade" totalsRowDxfId="132" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S5.2[[#This Row],[Mark]]="","",IF(AND(LEN(S5.2[[#This Row],[Course Code]])=10, S5.2[[#This Row],[Mark]]&gt;=60),"C",IF(S5.2[[#This Row],[Mark]]&lt;40,"F",IF(S5.2[[#This Row],[Mark]]&lt;45,"E",IF(S5.2[[#This Row],[Mark]]&lt;50,"D",IF(S5.2[[#This Row],[Mark]]&lt;60,"C",IF(S5.2[[#This Row],[Mark]]&lt;70,"B",IF(S5.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{2E68D5CE-4D79-4A9E-9ADB-A24E2CBA0A46}" name="GP" totalsRowDxfId="120" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{2E68D5CE-4D79-4A9E-9ADB-A24E2CBA0A46}" name="GP" totalsRowDxfId="131" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S5.2[[#This Row],[Mark]]="","",IF(AND(LEN(S5.2[[#This Row],[Course Code]])=10, S5.2[[#This Row],[Mark]]&gt;=60),3,IF(S5.2[[#This Row],[Mark]]&lt;40,0,IF(S5.2[[#This Row],[Mark]]&lt;45,1,IF(S5.2[[#This Row],[Mark]]&lt;50,2,IF(S5.2[[#This Row],[Mark]]&lt;60,3,IF(S5.2[[#This Row],[Mark]]&lt;70,4,IF(S5.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6B212538-FD03-4DE2-A613-AC39CABEAB26}" name="QP" totalsRowFunction="sum" totalsRowDxfId="119" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{6B212538-FD03-4DE2-A613-AC39CABEAB26}" name="QP" totalsRowFunction="sum" totalsRowDxfId="130" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S5.2[[#This Row],[CU]]*S5.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5257,20 +5497,20 @@
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5260D677-50C4-4608-AB66-B6ABABFBE5F1}" name="S6.1" displayName="S6.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="118" dataDxfId="117" totalsRowDxfId="116">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{5260D677-50C4-4608-AB66-B6ABABFBE5F1}" name="S6.1" displayName="S6.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="129" dataDxfId="128" totalsRowDxfId="127">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{12E9A3F6-94AF-4A85-828B-2817BCA9F2B8}" name="Course Code" totalsRowLabel="Total" dataDxfId="115" totalsRowDxfId="114"/>
-    <tableColumn id="2" xr3:uid="{1BD1A68B-9652-4CE3-BA4B-7C49ABE63B87}" name="Course Title" dataDxfId="113" totalsRowDxfId="112"/>
-    <tableColumn id="3" xr3:uid="{AE780C7B-44A9-4CC6-B40D-2D2526BDB6FC}" name="CU" totalsRowFunction="sum" totalsRowDxfId="111" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{A621E7EB-49AE-44E0-BF3C-EEAF6BFFD9F7}" name="Mark" totalsRowDxfId="110" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{AFD7290B-4CD9-40DB-A716-8DE4B81DBAAC}" name="Grade" totalsRowDxfId="109" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{12E9A3F6-94AF-4A85-828B-2817BCA9F2B8}" name="Course Code" totalsRowLabel="Total" dataDxfId="126" totalsRowDxfId="125"/>
+    <tableColumn id="2" xr3:uid="{1BD1A68B-9652-4CE3-BA4B-7C49ABE63B87}" name="Course Title" dataDxfId="124" totalsRowDxfId="123"/>
+    <tableColumn id="3" xr3:uid="{AE780C7B-44A9-4CC6-B40D-2D2526BDB6FC}" name="CU" totalsRowFunction="sum" totalsRowDxfId="122" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{A621E7EB-49AE-44E0-BF3C-EEAF6BFFD9F7}" name="Mark" totalsRowDxfId="121" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{AFD7290B-4CD9-40DB-A716-8DE4B81DBAAC}" name="Grade" totalsRowDxfId="120" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S6.1[[#This Row],[Mark]]="","",IF(AND(LEN(S6.1[[#This Row],[Course Code]])=10, S6.1[[#This Row],[Mark]]&gt;=60),"C",IF(S6.1[[#This Row],[Mark]]&lt;40,"F",IF(S6.1[[#This Row],[Mark]]&lt;45,"E",IF(S6.1[[#This Row],[Mark]]&lt;50,"D",IF(S6.1[[#This Row],[Mark]]&lt;60,"C",IF(S6.1[[#This Row],[Mark]]&lt;70,"B",IF(S6.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{839C19EA-45B4-414C-A1D8-D3355F81FA7E}" name="GP" totalsRowDxfId="108" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{839C19EA-45B4-414C-A1D8-D3355F81FA7E}" name="GP" totalsRowDxfId="119" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S6.1[[#This Row],[Mark]]="","",IF(AND(LEN(S6.1[[#This Row],[Course Code]])=10, S6.1[[#This Row],[Mark]]&gt;=60),3,IF(S6.1[[#This Row],[Mark]]&lt;40,0,IF(S6.1[[#This Row],[Mark]]&lt;45,1,IF(S6.1[[#This Row],[Mark]]&lt;50,2,IF(S6.1[[#This Row],[Mark]]&lt;60,3,IF(S6.1[[#This Row],[Mark]]&lt;70,4,IF(S6.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6B03D6DF-AC00-4946-875F-9579D40E2252}" name="QP" totalsRowFunction="sum" totalsRowDxfId="107" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{6B03D6DF-AC00-4946-875F-9579D40E2252}" name="QP" totalsRowFunction="sum" totalsRowDxfId="118" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S6.1[[#This Row],[CU]]*S6.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5279,20 +5519,20 @@
 </file>
 
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{16CC985D-7D9D-4805-8990-0F4D40A24713}" name="S6.2" displayName="S6.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="106" dataDxfId="105" totalsRowDxfId="104">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="12" xr:uid="{16CC985D-7D9D-4805-8990-0F4D40A24713}" name="S6.2" displayName="S6.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="117" dataDxfId="116" totalsRowDxfId="115">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{73AE99F9-4D7E-4EE8-BB6E-0AE281DD2012}" name="Course Code" totalsRowLabel="Total" dataDxfId="103" totalsRowDxfId="102"/>
-    <tableColumn id="2" xr3:uid="{E5FE2EC1-C8D6-44F5-8629-4A837DA729BE}" name="Course Title" dataDxfId="101" totalsRowDxfId="100"/>
-    <tableColumn id="3" xr3:uid="{3B1623F2-7092-4305-B147-A550A7CC4D0A}" name="CU" totalsRowFunction="sum" totalsRowDxfId="99" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{4EA59991-8A15-4268-A2FD-A85BA19753D3}" name="Mark" totalsRowDxfId="98" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{784E853E-621F-456F-B3DA-A17B6FA82767}" name="Grade" totalsRowDxfId="97" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{73AE99F9-4D7E-4EE8-BB6E-0AE281DD2012}" name="Course Code" totalsRowLabel="Total" dataDxfId="114" totalsRowDxfId="113"/>
+    <tableColumn id="2" xr3:uid="{E5FE2EC1-C8D6-44F5-8629-4A837DA729BE}" name="Course Title" dataDxfId="112" totalsRowDxfId="111"/>
+    <tableColumn id="3" xr3:uid="{3B1623F2-7092-4305-B147-A550A7CC4D0A}" name="CU" totalsRowFunction="sum" totalsRowDxfId="110" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{4EA59991-8A15-4268-A2FD-A85BA19753D3}" name="Mark" totalsRowDxfId="109" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{784E853E-621F-456F-B3DA-A17B6FA82767}" name="Grade" totalsRowDxfId="108" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S6.2[[#This Row],[Mark]]="","",IF(AND(LEN(S6.2[[#This Row],[Course Code]])=10, S6.2[[#This Row],[Mark]]&gt;=60),"C",IF(S6.2[[#This Row],[Mark]]&lt;40,"F",IF(S6.2[[#This Row],[Mark]]&lt;45,"E",IF(S6.2[[#This Row],[Mark]]&lt;50,"D",IF(S6.2[[#This Row],[Mark]]&lt;60,"C",IF(S6.2[[#This Row],[Mark]]&lt;70,"B",IF(S6.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{B1B5AC62-B91D-4B4D-8884-2550C4391A8D}" name="GP" totalsRowDxfId="96" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{B1B5AC62-B91D-4B4D-8884-2550C4391A8D}" name="GP" totalsRowDxfId="107" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S6.2[[#This Row],[Mark]]="","",IF(AND(LEN(S6.2[[#This Row],[Course Code]])=10, S6.2[[#This Row],[Mark]]&gt;=60),3,IF(S6.2[[#This Row],[Mark]]&lt;40,0,IF(S6.2[[#This Row],[Mark]]&lt;45,1,IF(S6.2[[#This Row],[Mark]]&lt;50,2,IF(S6.2[[#This Row],[Mark]]&lt;60,3,IF(S6.2[[#This Row],[Mark]]&lt;70,4,IF(S6.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2B41BB85-F6E0-4CF2-90A5-151739442998}" name="QP" totalsRowFunction="sum" totalsRowDxfId="95" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{2B41BB85-F6E0-4CF2-90A5-151739442998}" name="QP" totalsRowFunction="sum" totalsRowDxfId="106" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S6.2[[#This Row],[CU]]*S6.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5301,20 +5541,20 @@
 </file>
 
 <file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{BD147B1C-9646-44DF-89BD-CA6F88CC8B76}" name="S7.1" displayName="S7.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="94" dataDxfId="93" totalsRowDxfId="92">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{BD147B1C-9646-44DF-89BD-CA6F88CC8B76}" name="S7.1" displayName="S7.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="105" dataDxfId="104" totalsRowDxfId="103">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{F8A74AC6-C3F2-4015-A663-C85E27A7D4A6}" name="Course Code" totalsRowLabel="Total" dataDxfId="91" totalsRowDxfId="90"/>
-    <tableColumn id="2" xr3:uid="{83043BE7-6F68-43B6-BC9E-875A1B5EBD52}" name="Course Title" dataDxfId="89" totalsRowDxfId="88"/>
-    <tableColumn id="3" xr3:uid="{6FD4E4E0-E0B8-49F2-AB26-91EDA3B5DFE2}" name="CU" totalsRowFunction="sum" totalsRowDxfId="87" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{06A77FBF-CA62-432A-BACB-02910EFA06B3}" name="Mark" totalsRowDxfId="86" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{0B007AB7-561B-4F48-9C4D-F7C62FD9FC1F}" name="Grade" totalsRowDxfId="85" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{F8A74AC6-C3F2-4015-A663-C85E27A7D4A6}" name="Course Code" totalsRowLabel="Total" dataDxfId="102" totalsRowDxfId="101"/>
+    <tableColumn id="2" xr3:uid="{83043BE7-6F68-43B6-BC9E-875A1B5EBD52}" name="Course Title" dataDxfId="100" totalsRowDxfId="99"/>
+    <tableColumn id="3" xr3:uid="{6FD4E4E0-E0B8-49F2-AB26-91EDA3B5DFE2}" name="CU" totalsRowFunction="sum" totalsRowDxfId="98" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{06A77FBF-CA62-432A-BACB-02910EFA06B3}" name="Mark" totalsRowDxfId="97" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{0B007AB7-561B-4F48-9C4D-F7C62FD9FC1F}" name="Grade" totalsRowDxfId="96" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S7.1[[#This Row],[Mark]]="","",IF(AND(LEN(S7.1[[#This Row],[Course Code]])=10, S7.1[[#This Row],[Mark]]&gt;=60),"C",IF(S7.1[[#This Row],[Mark]]&lt;40,"F",IF(S7.1[[#This Row],[Mark]]&lt;45,"E",IF(S7.1[[#This Row],[Mark]]&lt;50,"D",IF(S7.1[[#This Row],[Mark]]&lt;60,"C",IF(S7.1[[#This Row],[Mark]]&lt;70,"B",IF(S7.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{9FC2832D-CCCA-41A6-900E-2D404E28ADA1}" name="GP" totalsRowDxfId="84" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{9FC2832D-CCCA-41A6-900E-2D404E28ADA1}" name="GP" totalsRowDxfId="95" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S7.1[[#This Row],[Mark]]="","",IF(AND(LEN(S7.1[[#This Row],[Course Code]])=10, S7.1[[#This Row],[Mark]]&gt;=60),3,IF(S7.1[[#This Row],[Mark]]&lt;40,0,IF(S7.1[[#This Row],[Mark]]&lt;45,1,IF(S7.1[[#This Row],[Mark]]&lt;50,2,IF(S7.1[[#This Row],[Mark]]&lt;60,3,IF(S7.1[[#This Row],[Mark]]&lt;70,4,IF(S7.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{5BEA7D85-356F-404F-BD0F-8CCF189C70FE}" name="QP" totalsRowFunction="sum" totalsRowDxfId="83" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{5BEA7D85-356F-404F-BD0F-8CCF189C70FE}" name="QP" totalsRowFunction="sum" totalsRowDxfId="94" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S7.1[[#This Row],[CU]]*S7.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5323,20 +5563,20 @@
 </file>
 
 <file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AE0582CF-5DEA-4192-8D30-F1C779CFA286}" name="S7.2" displayName="S7.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="82" dataDxfId="81" totalsRowDxfId="80">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="14" xr:uid="{AE0582CF-5DEA-4192-8D30-F1C779CFA286}" name="S7.2" displayName="S7.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="93" dataDxfId="92" totalsRowDxfId="91">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{690339ED-09C4-4752-B333-0DC82C4140A4}" name="Course Code" totalsRowLabel="Total" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{AA305358-3BDF-4040-A6AE-702BEF6A4591}" name="Course Title" dataDxfId="77" totalsRowDxfId="76"/>
-    <tableColumn id="3" xr3:uid="{2479E734-480D-4B6D-B5D5-5FC474A8F0AB}" name="CU" totalsRowFunction="sum" totalsRowDxfId="75" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{50773009-2506-43E9-86E0-5D7FF51EB350}" name="Mark" totalsRowDxfId="74" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{0B6EF311-F7A5-40B1-BBDB-5AC5D4F4023D}" name="Grade" totalsRowDxfId="73" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{690339ED-09C4-4752-B333-0DC82C4140A4}" name="Course Code" totalsRowLabel="Total" dataDxfId="90" totalsRowDxfId="89"/>
+    <tableColumn id="2" xr3:uid="{AA305358-3BDF-4040-A6AE-702BEF6A4591}" name="Course Title" dataDxfId="88" totalsRowDxfId="87"/>
+    <tableColumn id="3" xr3:uid="{2479E734-480D-4B6D-B5D5-5FC474A8F0AB}" name="CU" totalsRowFunction="sum" totalsRowDxfId="86" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{50773009-2506-43E9-86E0-5D7FF51EB350}" name="Mark" totalsRowDxfId="85" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{0B6EF311-F7A5-40B1-BBDB-5AC5D4F4023D}" name="Grade" totalsRowDxfId="84" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S7.2[[#This Row],[Mark]]="","",IF(AND(LEN(S7.2[[#This Row],[Course Code]])=10, S7.2[[#This Row],[Mark]]&gt;=60),"C",IF(S7.2[[#This Row],[Mark]]&lt;40,"F",IF(S7.2[[#This Row],[Mark]]&lt;45,"E",IF(S7.2[[#This Row],[Mark]]&lt;50,"D",IF(S7.2[[#This Row],[Mark]]&lt;60,"C",IF(S7.2[[#This Row],[Mark]]&lt;70,"B",IF(S7.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{26D86D42-1427-4E1F-B7A2-8C4BA3BFBDCC}" name="GP" totalsRowDxfId="72" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{26D86D42-1427-4E1F-B7A2-8C4BA3BFBDCC}" name="GP" totalsRowDxfId="83" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S7.2[[#This Row],[Mark]]="","",IF(AND(LEN(S7.2[[#This Row],[Course Code]])=10, S7.2[[#This Row],[Mark]]&gt;=60),3,IF(S7.2[[#This Row],[Mark]]&lt;40,0,IF(S7.2[[#This Row],[Mark]]&lt;45,1,IF(S7.2[[#This Row],[Mark]]&lt;50,2,IF(S7.2[[#This Row],[Mark]]&lt;60,3,IF(S7.2[[#This Row],[Mark]]&lt;70,4,IF(S7.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{6E1E0B5F-E672-4EFB-9B59-C1DD0B97F14F}" name="QP" totalsRowFunction="sum" totalsRowDxfId="71" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{6E1E0B5F-E672-4EFB-9B59-C1DD0B97F14F}" name="QP" totalsRowFunction="sum" totalsRowDxfId="82" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S7.2[[#This Row],[CU]]*S7.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5345,20 +5585,20 @@
 </file>
 
 <file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{4CE8EF41-557C-436A-B1E0-4B804CE5681A}" name="S8.1" displayName="S8.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="70" dataDxfId="69" totalsRowDxfId="68">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="15" xr:uid="{4CE8EF41-557C-436A-B1E0-4B804CE5681A}" name="S8.1" displayName="S8.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="81" dataDxfId="80" totalsRowDxfId="79">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{7A795FE8-13CD-4053-AE14-EAB29EDCD1CF}" name="Course Code" totalsRowLabel="Total" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="2" xr3:uid="{C9D7CDA2-2330-432B-B37B-722BDB6A054B}" name="Course Title" dataDxfId="65" totalsRowDxfId="64"/>
-    <tableColumn id="3" xr3:uid="{41F3D526-ABE0-445B-9079-69040DAFE0CC}" name="CU" totalsRowFunction="sum" totalsRowDxfId="63" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{CD6685EC-D1B3-460C-9FAA-07741662A447}" name="Mark" totalsRowDxfId="62" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{ECCB9EC2-C08B-4EDB-83F5-DADDE681815B}" name="Grade" totalsRowDxfId="61" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{7A795FE8-13CD-4053-AE14-EAB29EDCD1CF}" name="Course Code" totalsRowLabel="Total" dataDxfId="78" totalsRowDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{C9D7CDA2-2330-432B-B37B-722BDB6A054B}" name="Course Title" dataDxfId="76" totalsRowDxfId="75"/>
+    <tableColumn id="3" xr3:uid="{41F3D526-ABE0-445B-9079-69040DAFE0CC}" name="CU" totalsRowFunction="sum" totalsRowDxfId="74" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{CD6685EC-D1B3-460C-9FAA-07741662A447}" name="Mark" totalsRowDxfId="73" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{ECCB9EC2-C08B-4EDB-83F5-DADDE681815B}" name="Grade" totalsRowDxfId="72" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S8.1[[#This Row],[Mark]]="","",IF(AND(LEN(S8.1[[#This Row],[Course Code]])=10, S8.1[[#This Row],[Mark]]&gt;=60),"C",IF(S8.1[[#This Row],[Mark]]&lt;40,"F",IF(S8.1[[#This Row],[Mark]]&lt;45,"E",IF(S8.1[[#This Row],[Mark]]&lt;50,"D",IF(S8.1[[#This Row],[Mark]]&lt;60,"C",IF(S8.1[[#This Row],[Mark]]&lt;70,"B",IF(S8.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C7D08A16-B520-4E08-9AFE-BE109BFAF65E}" name="GP" totalsRowDxfId="60" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{C7D08A16-B520-4E08-9AFE-BE109BFAF65E}" name="GP" totalsRowDxfId="71" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S8.1[[#This Row],[Mark]]="","",IF(AND(LEN(S8.1[[#This Row],[Course Code]])=10, S8.1[[#This Row],[Mark]]&gt;=60),3,IF(S8.1[[#This Row],[Mark]]&lt;40,0,IF(S8.1[[#This Row],[Mark]]&lt;45,1,IF(S8.1[[#This Row],[Mark]]&lt;50,2,IF(S8.1[[#This Row],[Mark]]&lt;60,3,IF(S8.1[[#This Row],[Mark]]&lt;70,4,IF(S8.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{2ABBE079-F661-4A7B-968F-7BE25D948E21}" name="QP" totalsRowFunction="sum" totalsRowDxfId="59" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{2ABBE079-F661-4A7B-968F-7BE25D948E21}" name="QP" totalsRowFunction="sum" totalsRowDxfId="70" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S8.1[[#This Row],[CU]]*S8.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5367,20 +5607,20 @@
 </file>
 
 <file path=xl/tables/table16.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{B55E716E-AF2D-4C41-8703-02D42CFDB798}" name="S8.2" displayName="S8.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="58" dataDxfId="57" totalsRowDxfId="56">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="16" xr:uid="{B55E716E-AF2D-4C41-8703-02D42CFDB798}" name="S8.2" displayName="S8.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="69" dataDxfId="68" totalsRowDxfId="67">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{6BEF9D2B-8A40-4CCE-99F5-52EF0CA44DAA}" name="Course Code" totalsRowLabel="Total" dataDxfId="55" totalsRowDxfId="54"/>
-    <tableColumn id="2" xr3:uid="{C5FA9B04-CBC2-4A7B-91C0-8A5952CFC8F3}" name="Course Title" dataDxfId="53" totalsRowDxfId="52"/>
-    <tableColumn id="3" xr3:uid="{F6F1DBD2-CA5F-467D-A480-A14D0972ADFB}" name="CU" totalsRowFunction="sum" totalsRowDxfId="51" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{BBB8A3CC-AC7B-45AD-B3B5-4C47F1470F5B}" name="Mark" totalsRowDxfId="50" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{E127A250-7450-461B-BC09-F219EA8A77E2}" name="Grade" totalsRowDxfId="49" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{6BEF9D2B-8A40-4CCE-99F5-52EF0CA44DAA}" name="Course Code" totalsRowLabel="Total" dataDxfId="66" totalsRowDxfId="65"/>
+    <tableColumn id="2" xr3:uid="{C5FA9B04-CBC2-4A7B-91C0-8A5952CFC8F3}" name="Course Title" dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="3" xr3:uid="{F6F1DBD2-CA5F-467D-A480-A14D0972ADFB}" name="CU" totalsRowFunction="sum" totalsRowDxfId="62" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{BBB8A3CC-AC7B-45AD-B3B5-4C47F1470F5B}" name="Mark" totalsRowDxfId="61" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{E127A250-7450-461B-BC09-F219EA8A77E2}" name="Grade" totalsRowDxfId="60" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S8.2[[#This Row],[Mark]]="","",IF(AND(LEN(S8.2[[#This Row],[Course Code]])=10, S8.2[[#This Row],[Mark]]&gt;=60),"C",IF(S8.2[[#This Row],[Mark]]&lt;40,"F",IF(S8.2[[#This Row],[Mark]]&lt;45,"E",IF(S8.2[[#This Row],[Mark]]&lt;50,"D",IF(S8.2[[#This Row],[Mark]]&lt;60,"C",IF(S8.2[[#This Row],[Mark]]&lt;70,"B",IF(S8.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F36A54AB-CF05-41F7-8407-36F3F34705C6}" name="GP" totalsRowDxfId="48" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{F36A54AB-CF05-41F7-8407-36F3F34705C6}" name="GP" totalsRowDxfId="59" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S8.2[[#This Row],[Mark]]="","",IF(AND(LEN(S8.2[[#This Row],[Course Code]])=10, S8.2[[#This Row],[Mark]]&gt;=60),3,IF(S8.2[[#This Row],[Mark]]&lt;40,0,IF(S8.2[[#This Row],[Mark]]&lt;45,1,IF(S8.2[[#This Row],[Mark]]&lt;50,2,IF(S8.2[[#This Row],[Mark]]&lt;60,3,IF(S8.2[[#This Row],[Mark]]&lt;70,4,IF(S8.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{40D8A475-EF07-4F5D-BC7D-2E8E4F517C42}" name="QP" totalsRowFunction="sum" totalsRowDxfId="47" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{40D8A475-EF07-4F5D-BC7D-2E8E4F517C42}" name="QP" totalsRowFunction="sum" totalsRowDxfId="58" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S8.2[[#This Row],[CU]]*S8.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5389,20 +5629,20 @@
 </file>
 
 <file path=xl/tables/table17.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{0BFD61BA-B765-43D8-AEA3-0C40E7E08345}" name="S9.1" displayName="S9.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="46" dataDxfId="45" totalsRowDxfId="44">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="17" xr:uid="{0BFD61BA-B765-43D8-AEA3-0C40E7E08345}" name="S9.1" displayName="S9.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="57" dataDxfId="56" totalsRowDxfId="55">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{611833D2-E9D8-4E1D-AFBC-C8A594412AAF}" name="Course Code" totalsRowLabel="Total" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="2" xr3:uid="{667B4E24-AEF7-4E3B-858C-D5547074A8F8}" name="Course Title" dataDxfId="41" totalsRowDxfId="40"/>
-    <tableColumn id="3" xr3:uid="{8AF93E9D-B07D-4CAA-8639-26E162BF6503}" name="CU" totalsRowFunction="sum" totalsRowDxfId="39" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{135BCF47-8A08-4233-BA68-A991ADDBD241}" name="Mark" totalsRowDxfId="38" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{7DC78208-2225-4B03-87DC-FE6E859D19D6}" name="Grade" totalsRowDxfId="37" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{611833D2-E9D8-4E1D-AFBC-C8A594412AAF}" name="Course Code" totalsRowLabel="Total" dataDxfId="54" totalsRowDxfId="53"/>
+    <tableColumn id="2" xr3:uid="{667B4E24-AEF7-4E3B-858C-D5547074A8F8}" name="Course Title" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="3" xr3:uid="{8AF93E9D-B07D-4CAA-8639-26E162BF6503}" name="CU" totalsRowFunction="sum" totalsRowDxfId="50" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{135BCF47-8A08-4233-BA68-A991ADDBD241}" name="Mark" totalsRowDxfId="49" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{7DC78208-2225-4B03-87DC-FE6E859D19D6}" name="Grade" totalsRowDxfId="48" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S9.1[[#This Row],[Mark]]="","",IF(AND(LEN(S9.1[[#This Row],[Course Code]])=10, S9.1[[#This Row],[Mark]]&gt;=60),"C",IF(S9.1[[#This Row],[Mark]]&lt;40,"F",IF(S9.1[[#This Row],[Mark]]&lt;45,"E",IF(S9.1[[#This Row],[Mark]]&lt;50,"D",IF(S9.1[[#This Row],[Mark]]&lt;60,"C",IF(S9.1[[#This Row],[Mark]]&lt;70,"B",IF(S9.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E32E0B5E-7571-4D2B-A511-A02C2E9CC99E}" name="GP" totalsRowDxfId="36" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{E32E0B5E-7571-4D2B-A511-A02C2E9CC99E}" name="GP" totalsRowDxfId="47" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S9.1[[#This Row],[Mark]]="","",IF(AND(LEN(S9.1[[#This Row],[Course Code]])=10, S9.1[[#This Row],[Mark]]&gt;=60),3,IF(S9.1[[#This Row],[Mark]]&lt;40,0,IF(S9.1[[#This Row],[Mark]]&lt;45,1,IF(S9.1[[#This Row],[Mark]]&lt;50,2,IF(S9.1[[#This Row],[Mark]]&lt;60,3,IF(S9.1[[#This Row],[Mark]]&lt;70,4,IF(S9.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{3C0BE365-5392-436F-8F40-91C377720568}" name="QP" totalsRowFunction="sum" totalsRowDxfId="35" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{3C0BE365-5392-436F-8F40-91C377720568}" name="QP" totalsRowFunction="sum" totalsRowDxfId="46" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S9.1[[#This Row],[CU]]*S9.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5411,20 +5651,20 @@
 </file>
 
 <file path=xl/tables/table18.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{ADE0DB04-E1DD-4524-8553-ABBFA03C556C}" name="S9.2" displayName="S9.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="34" dataDxfId="33" totalsRowDxfId="32">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="18" xr:uid="{ADE0DB04-E1DD-4524-8553-ABBFA03C556C}" name="S9.2" displayName="S9.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="45" dataDxfId="44" totalsRowDxfId="43">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A995B81D-6C36-410F-B499-BBFE40A0CAF0}" name="Course Code" totalsRowLabel="Total" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="2" xr3:uid="{64D4BFBA-DE7D-4398-879B-167FA554C2CD}" name="Course Title" dataDxfId="29" totalsRowDxfId="28"/>
-    <tableColumn id="3" xr3:uid="{08C214A8-EDDE-4946-8287-975C944D7F6A}" name="CU" totalsRowFunction="sum" totalsRowDxfId="27" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{4DDC32FB-19D8-4731-AE3A-D57B6CFA05F6}" name="Mark" totalsRowDxfId="26" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{F529D9E6-3774-4ACD-91B6-88BEF4530445}" name="Grade" totalsRowDxfId="25" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{A995B81D-6C36-410F-B499-BBFE40A0CAF0}" name="Course Code" totalsRowLabel="Total" dataDxfId="42" totalsRowDxfId="41"/>
+    <tableColumn id="2" xr3:uid="{64D4BFBA-DE7D-4398-879B-167FA554C2CD}" name="Course Title" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="3" xr3:uid="{08C214A8-EDDE-4946-8287-975C944D7F6A}" name="CU" totalsRowFunction="sum" totalsRowDxfId="38" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{4DDC32FB-19D8-4731-AE3A-D57B6CFA05F6}" name="Mark" totalsRowDxfId="37" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{F529D9E6-3774-4ACD-91B6-88BEF4530445}" name="Grade" totalsRowDxfId="36" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S9.2[[#This Row],[Mark]]="","",IF(AND(LEN(S9.2[[#This Row],[Course Code]])=10, S9.2[[#This Row],[Mark]]&gt;=60),"C",IF(S9.2[[#This Row],[Mark]]&lt;40,"F",IF(S9.2[[#This Row],[Mark]]&lt;45,"E",IF(S9.2[[#This Row],[Mark]]&lt;50,"D",IF(S9.2[[#This Row],[Mark]]&lt;60,"C",IF(S9.2[[#This Row],[Mark]]&lt;70,"B",IF(S9.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{341F371A-EC55-4312-9F72-A27EA4163379}" name="GP" totalsRowDxfId="24" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{341F371A-EC55-4312-9F72-A27EA4163379}" name="GP" totalsRowDxfId="35" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S9.2[[#This Row],[Mark]]="","",IF(AND(LEN(S9.2[[#This Row],[Course Code]])=10, S9.2[[#This Row],[Mark]]&gt;=60),3,IF(S9.2[[#This Row],[Mark]]&lt;40,0,IF(S9.2[[#This Row],[Mark]]&lt;45,1,IF(S9.2[[#This Row],[Mark]]&lt;50,2,IF(S9.2[[#This Row],[Mark]]&lt;60,3,IF(S9.2[[#This Row],[Mark]]&lt;70,4,IF(S9.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{C14D31C3-4A04-45F0-BD43-5EB19341EDA1}" name="QP" totalsRowFunction="sum" totalsRowDxfId="23" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{C14D31C3-4A04-45F0-BD43-5EB19341EDA1}" name="QP" totalsRowFunction="sum" totalsRowDxfId="34" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S9.2[[#This Row],[CU]]*S9.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5433,38 +5673,38 @@
 </file>
 
 <file path=xl/tables/table19.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{4DE29814-387D-4E88-AB23-8407891F81F2}" name="Flagged" displayName="Flagged" ref="A10:G12" totalsRowCount="1" headerRowDxfId="22" dataDxfId="21" totalsRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="20" xr:uid="{4DE29814-387D-4E88-AB23-8407891F81F2}" name="Flagged" displayName="Flagged" ref="A10:G12" totalsRowCount="1" headerRowDxfId="33" dataDxfId="32" totalsRowDxfId="31">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{944EB04F-1BD9-42F7-8770-84EFBDC079AD}" name="Course Code" totalsRowLabel="Total" dataDxfId="19" totalsRowDxfId="18"/>
-    <tableColumn id="2" xr3:uid="{C26D477F-198A-4820-BEF5-C85FB09034C9}" name="Course Title" dataDxfId="17" totalsRowDxfId="16"/>
-    <tableColumn id="3" xr3:uid="{128D06A2-BCDA-4F9E-BA7B-4220D5374792}" name="CU" totalsRowFunction="sum" totalsRowDxfId="15" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{6ADFF330-D98B-45E2-8412-66E7D0DDD828}" name="Mark" totalsRowDxfId="14" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{C1C184AC-DD32-47D9-A7FE-1D08956BA12A}" name="Grade" totalsRowDxfId="13" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{944EB04F-1BD9-42F7-8770-84EFBDC079AD}" name="Course Code" totalsRowLabel="Total" dataDxfId="30" totalsRowDxfId="29"/>
+    <tableColumn id="2" xr3:uid="{C26D477F-198A-4820-BEF5-C85FB09034C9}" name="Course Title" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="3" xr3:uid="{128D06A2-BCDA-4F9E-BA7B-4220D5374792}" name="CU" totalsRowFunction="sum" totalsRowDxfId="26" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{6ADFF330-D98B-45E2-8412-66E7D0DDD828}" name="Mark" totalsRowDxfId="25" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{C1C184AC-DD32-47D9-A7FE-1D08956BA12A}" name="Grade" totalsRowDxfId="24" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(Flagged[[#This Row],[Mark]]="","",IF(AND(LEN(Flagged[[#This Row],[Course Code]])=10, Flagged[[#This Row],[Mark]]&gt;=60),"C",IF(Flagged[[#This Row],[Mark]]&lt;40,"F",IF(Flagged[[#This Row],[Mark]]&lt;45,"E",IF(Flagged[[#This Row],[Mark]]&lt;50,"D",IF(Flagged[[#This Row],[Mark]]&lt;60,"C",IF(Flagged[[#This Row],[Mark]]&lt;70,"B",IF(Flagged[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{C792FA37-5431-40E6-B8D7-5AF59CBE55D7}" name="Session" totalsRowDxfId="12" dataCellStyle="Number Style"/>
-    <tableColumn id="7" xr3:uid="{C62DA4E8-E108-42E6-A0AA-53F1BCCF6CD9}" name="Reason" totalsRowDxfId="11" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{C792FA37-5431-40E6-B8D7-5AF59CBE55D7}" name="Session" totalsRowDxfId="23" dataCellStyle="Number Style"/>
+    <tableColumn id="7" xr3:uid="{C62DA4E8-E108-42E6-A0AA-53F1BCCF6CD9}" name="Reason" totalsRowDxfId="22" dataCellStyle="Normal"/>
   </tableColumns>
   <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C6E48F7B-C7FF-4EBC-93DE-3EBBA7AE9EE2}" name="S1.2" displayName="S1.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="226" dataDxfId="225" totalsRowDxfId="224">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C6E48F7B-C7FF-4EBC-93DE-3EBBA7AE9EE2}" name="S1.2" displayName="S1.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="237" dataDxfId="236" totalsRowDxfId="235">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{3F94AFDB-431F-43FB-9A1A-8F156DBEF053}" name="Course Code" totalsRowLabel="Total" dataDxfId="223" totalsRowDxfId="222"/>
-    <tableColumn id="2" xr3:uid="{1B03271A-ABC1-4B85-BDED-0C56B7703ECE}" name="Course Title" dataDxfId="221" totalsRowDxfId="220"/>
-    <tableColumn id="3" xr3:uid="{A4651DAB-C035-4FE2-AD35-47765D8074D5}" name="CU" totalsRowFunction="sum" totalsRowDxfId="219" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{A7DEF8C9-33A1-4FE3-B09E-95CF9D9B3D31}" name="Mark" totalsRowDxfId="218" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{38CB5DE5-D190-40D7-BA36-9228B7AEDCCA}" name="Grade" totalsRowDxfId="217" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{3F94AFDB-431F-43FB-9A1A-8F156DBEF053}" name="Course Code" totalsRowLabel="Total" dataDxfId="234" totalsRowDxfId="233"/>
+    <tableColumn id="2" xr3:uid="{1B03271A-ABC1-4B85-BDED-0C56B7703ECE}" name="Course Title" dataDxfId="232" totalsRowDxfId="231"/>
+    <tableColumn id="3" xr3:uid="{A4651DAB-C035-4FE2-AD35-47765D8074D5}" name="CU" totalsRowFunction="sum" totalsRowDxfId="230" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{A7DEF8C9-33A1-4FE3-B09E-95CF9D9B3D31}" name="Mark" totalsRowDxfId="229" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{38CB5DE5-D190-40D7-BA36-9228B7AEDCCA}" name="Grade" totalsRowDxfId="228" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S1.2[[#This Row],[Mark]]="","",IF(AND(LEN(S1.2[[#This Row],[Course Code]])=10, S1.2[[#This Row],[Mark]]&gt;=60),"C",IF(S1.2[[#This Row],[Mark]]&lt;40,"F",IF(S1.2[[#This Row],[Mark]]&lt;45,"E",IF(S1.2[[#This Row],[Mark]]&lt;50,"D",IF(S1.2[[#This Row],[Mark]]&lt;60,"C",IF(S1.2[[#This Row],[Mark]]&lt;70,"B",IF(S1.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{07962B54-CB9F-4D8B-B98B-11246A0F4124}" name="GP" totalsRowDxfId="216" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{07962B54-CB9F-4D8B-B98B-11246A0F4124}" name="GP" totalsRowDxfId="227" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S1.2[[#This Row],[Mark]]="","",IF(AND(LEN(S1.2[[#This Row],[Course Code]])=10, S1.2[[#This Row],[Mark]]&gt;=60),3,IF(S1.2[[#This Row],[Mark]]&lt;40,0,IF(S1.2[[#This Row],[Mark]]&lt;45,1,IF(S1.2[[#This Row],[Mark]]&lt;50,2,IF(S1.2[[#This Row],[Mark]]&lt;60,3,IF(S1.2[[#This Row],[Mark]]&lt;70,4,IF(S1.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{230D538B-9A76-4C0F-BD92-D86A8AEF5FEE}" name="QP" totalsRowFunction="sum" totalsRowDxfId="215" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{230D538B-9A76-4C0F-BD92-D86A8AEF5FEE}" name="QP" totalsRowFunction="sum" totalsRowDxfId="226" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S1.2[[#This Row],[CU]]*S1.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5473,37 +5713,54 @@
 </file>
 
 <file path=xl/tables/table20.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{04B5BFC3-8AA9-427D-8CF3-80475AFDC6F5}" name="Unknown" displayName="Unknown" ref="A10:F12" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="19" xr:uid="{04B5BFC3-8AA9-427D-8CF3-80475AFDC6F5}" name="Unknown" displayName="Unknown" ref="A10:F12" totalsRowCount="1" headerRowDxfId="21" dataDxfId="20" totalsRowDxfId="19">
   <autoFilter ref="A10:F11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{76D571A1-3DFE-47CD-9113-AD850BC06622}" name="Course Code" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C6F77A54-E001-4630-A19B-A21D9D2F0F20}" name="Course Title" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="3" xr3:uid="{1998C348-2D03-4F42-80A1-BC05E3A48BC1}" name="CU" totalsRowFunction="sum" totalsRowDxfId="3" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{3FD1F606-8400-4AB0-8EF7-490910A85DF9}" name="Mark" totalsRowDxfId="2" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{AFFE1CA0-63C6-4DB6-AC76-A3C8D5D4C4D0}" name="Grade" totalsRowDxfId="1" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{76D571A1-3DFE-47CD-9113-AD850BC06622}" name="Course Code" totalsRowLabel="Total" dataDxfId="18" totalsRowDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{C6F77A54-E001-4630-A19B-A21D9D2F0F20}" name="Course Title" dataDxfId="16" totalsRowDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{1998C348-2D03-4F42-80A1-BC05E3A48BC1}" name="CU" totalsRowFunction="sum" totalsRowDxfId="14" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{3FD1F606-8400-4AB0-8EF7-490910A85DF9}" name="Mark" totalsRowDxfId="13" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{AFFE1CA0-63C6-4DB6-AC76-A3C8D5D4C4D0}" name="Grade" totalsRowDxfId="12" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(Unknown[[#This Row],[Mark]]="","",IF(AND(LEN(Unknown[[#This Row],[Course Code]])=10, Unknown[[#This Row],[Mark]]&gt;=60),"C",IF(Unknown[[#This Row],[Mark]]&lt;40,"F",IF(Unknown[[#This Row],[Mark]]&lt;45,"E",IF(Unknown[[#This Row],[Mark]]&lt;50,"D",IF(Unknown[[#This Row],[Mark]]&lt;60,"C",IF(Unknown[[#This Row],[Mark]]&lt;70,"B",IF(Unknown[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{369200A6-41C9-4202-B715-3BA8130D59FA}" name="Session" totalsRowDxfId="0" dataCellStyle="Number Style"/>
+    <tableColumn id="6" xr3:uid="{369200A6-41C9-4202-B715-3BA8130D59FA}" name="Session" totalsRowDxfId="11" dataCellStyle="Number Style"/>
+  </tableColumns>
+  <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table21.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="21" xr:uid="{4AFEA5BD-081D-4114-9BD1-56D64A1649B5}" name="Outstanding" displayName="Outstanding" ref="A10:F12" totalsRowCount="1" headerRowDxfId="10" dataDxfId="9" totalsRowDxfId="8">
+  <autoFilter ref="A10:F11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
+  <tableColumns count="6">
+    <tableColumn id="1" xr3:uid="{53CAE1DB-B4C9-4295-A1AF-C3917FDC08CC}" name="Course Code" totalsRowLabel="Total" dataDxfId="7" totalsRowDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{2B28E97A-5695-45A7-BD6A-30E7828C0983}" name="Course Title" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{C86745FD-5E7E-4C9C-8781-45CEE71D909F}" name="CU" totalsRowFunction="sum" totalsRowDxfId="3" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{BA1862C5-2BF4-4E48-9DCF-71EB99CE6CE9}" name="Mark" totalsRowDxfId="2" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{7F6B53D5-5EBB-4970-842B-0590A23FE321}" name="Grade" totalsRowDxfId="1" dataCellStyle="Number Style">
+      <calculatedColumnFormula>IF(Outstanding[[#This Row],[Mark]]="","",IF(AND(LEN(Outstanding[[#This Row],[Course Code]])=10, Outstanding[[#This Row],[Mark]]&gt;=60),"C",IF(Outstanding[[#This Row],[Mark]]&lt;40,"F",IF(Outstanding[[#This Row],[Mark]]&lt;45,"E",IF(Outstanding[[#This Row],[Mark]]&lt;50,"D",IF(Outstanding[[#This Row],[Mark]]&lt;60,"C",IF(Outstanding[[#This Row],[Mark]]&lt;70,"B",IF(Outstanding[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="6" xr3:uid="{FB7DB57D-3786-4BD7-B910-264FB1FA37D1}" name="Session" totalsRowDxfId="0" dataCellStyle="Number Style"/>
   </tableColumns>
   <tableStyleInfo name="Semester Style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B68F9649-285F-4F79-8790-BCC0D91CBAD5}" name="S2.1" displayName="S2.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="214" dataDxfId="213" totalsRowDxfId="212">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{B68F9649-285F-4F79-8790-BCC0D91CBAD5}" name="S2.1" displayName="S2.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="225" dataDxfId="224" totalsRowDxfId="223">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1545C86C-14C2-45FD-B84E-8BF4E7D2C4A3}" name="Course Code" totalsRowLabel="Total" dataDxfId="211" totalsRowDxfId="210"/>
-    <tableColumn id="2" xr3:uid="{8C8D2FDE-5B53-4189-945D-FACD49C1A8A7}" name="Course Title" dataDxfId="209" totalsRowDxfId="208"/>
-    <tableColumn id="3" xr3:uid="{7EA0EB43-3029-4A4D-B786-EFA69C841EDD}" name="CU" totalsRowFunction="sum" totalsRowDxfId="207" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{A7B8C2F1-15A8-42D5-BD6E-C644E98B26B7}" name="Mark" totalsRowDxfId="206" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{6557EE38-7232-4B4B-A38E-2B7AA4B732AA}" name="Grade" totalsRowDxfId="205" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{1545C86C-14C2-45FD-B84E-8BF4E7D2C4A3}" name="Course Code" totalsRowLabel="Total" dataDxfId="222" totalsRowDxfId="221"/>
+    <tableColumn id="2" xr3:uid="{8C8D2FDE-5B53-4189-945D-FACD49C1A8A7}" name="Course Title" dataDxfId="220" totalsRowDxfId="219"/>
+    <tableColumn id="3" xr3:uid="{7EA0EB43-3029-4A4D-B786-EFA69C841EDD}" name="CU" totalsRowFunction="sum" totalsRowDxfId="218" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{A7B8C2F1-15A8-42D5-BD6E-C644E98B26B7}" name="Mark" totalsRowDxfId="217" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{6557EE38-7232-4B4B-A38E-2B7AA4B732AA}" name="Grade" totalsRowDxfId="216" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S2.1[[#This Row],[Mark]]="","",IF(AND(LEN(S2.1[[#This Row],[Course Code]])=10, S2.1[[#This Row],[Mark]]&gt;=60),"C",IF(S2.1[[#This Row],[Mark]]&lt;40,"F",IF(S2.1[[#This Row],[Mark]]&lt;45,"E",IF(S2.1[[#This Row],[Mark]]&lt;50,"D",IF(S2.1[[#This Row],[Mark]]&lt;60,"C",IF(S2.1[[#This Row],[Mark]]&lt;70,"B",IF(S2.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{02C02D78-1D37-45D0-BAB0-2933122865AB}" name="GP" totalsRowDxfId="204" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{02C02D78-1D37-45D0-BAB0-2933122865AB}" name="GP" totalsRowDxfId="215" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S2.1[[#This Row],[Mark]]="","",IF(AND(LEN(S2.1[[#This Row],[Course Code]])=10, S2.1[[#This Row],[Mark]]&gt;=60),3,IF(S2.1[[#This Row],[Mark]]&lt;40,0,IF(S2.1[[#This Row],[Mark]]&lt;45,1,IF(S2.1[[#This Row],[Mark]]&lt;50,2,IF(S2.1[[#This Row],[Mark]]&lt;60,3,IF(S2.1[[#This Row],[Mark]]&lt;70,4,IF(S2.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{99E31274-D711-49E5-97BB-7BDEBCE7C62E}" name="QP" totalsRowFunction="sum" totalsRowDxfId="203" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{99E31274-D711-49E5-97BB-7BDEBCE7C62E}" name="QP" totalsRowFunction="sum" totalsRowDxfId="214" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S2.1[[#This Row],[CU]]*S2.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5512,20 +5769,20 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{320AC645-3B4F-4868-9884-58AED04D9332}" name="S2.2" displayName="S2.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="202" dataDxfId="201" totalsRowDxfId="200">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{320AC645-3B4F-4868-9884-58AED04D9332}" name="S2.2" displayName="S2.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="213" dataDxfId="212" totalsRowDxfId="211">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B5A07E8E-F3BE-4048-AA35-25818CB3F400}" name="Course Code" totalsRowLabel="Total" dataDxfId="199" totalsRowDxfId="198"/>
-    <tableColumn id="2" xr3:uid="{610ABEB2-82F4-464C-8CEF-30F059DC0292}" name="Course Title" dataDxfId="197" totalsRowDxfId="196"/>
-    <tableColumn id="3" xr3:uid="{1E0559C5-69BA-437E-A760-649DE4F2B13C}" name="CU" totalsRowFunction="sum" totalsRowDxfId="195" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{CCE0BF4E-FB2C-4204-B0D0-8B0FD624A5BE}" name="Mark" totalsRowDxfId="194" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{0CF3CEF4-3CF7-451F-A392-2A6742592B48}" name="Grade" totalsRowDxfId="193" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{B5A07E8E-F3BE-4048-AA35-25818CB3F400}" name="Course Code" totalsRowLabel="Total" dataDxfId="210" totalsRowDxfId="209"/>
+    <tableColumn id="2" xr3:uid="{610ABEB2-82F4-464C-8CEF-30F059DC0292}" name="Course Title" dataDxfId="208" totalsRowDxfId="207"/>
+    <tableColumn id="3" xr3:uid="{1E0559C5-69BA-437E-A760-649DE4F2B13C}" name="CU" totalsRowFunction="sum" totalsRowDxfId="206" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{CCE0BF4E-FB2C-4204-B0D0-8B0FD624A5BE}" name="Mark" totalsRowDxfId="205" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{0CF3CEF4-3CF7-451F-A392-2A6742592B48}" name="Grade" totalsRowDxfId="204" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S2.2[[#This Row],[Mark]]="","",IF(AND(LEN(S2.2[[#This Row],[Course Code]])=10, S2.2[[#This Row],[Mark]]&gt;=60),"C",IF(S2.2[[#This Row],[Mark]]&lt;40,"F",IF(S2.2[[#This Row],[Mark]]&lt;45,"E",IF(S2.2[[#This Row],[Mark]]&lt;50,"D",IF(S2.2[[#This Row],[Mark]]&lt;60,"C",IF(S2.2[[#This Row],[Mark]]&lt;70,"B",IF(S2.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F39389A8-35CE-43AB-994B-EB6D64C43EAB}" name="GP" totalsRowDxfId="192" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{F39389A8-35CE-43AB-994B-EB6D64C43EAB}" name="GP" totalsRowDxfId="203" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S2.2[[#This Row],[Mark]]="","",IF(AND(LEN(S2.2[[#This Row],[Course Code]])=10, S2.2[[#This Row],[Mark]]&gt;=60),3,IF(S2.2[[#This Row],[Mark]]&lt;40,0,IF(S2.2[[#This Row],[Mark]]&lt;45,1,IF(S2.2[[#This Row],[Mark]]&lt;50,2,IF(S2.2[[#This Row],[Mark]]&lt;60,3,IF(S2.2[[#This Row],[Mark]]&lt;70,4,IF(S2.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{64EEA08C-5481-4401-BC85-B2556C39EB6B}" name="QP" totalsRowFunction="sum" totalsRowDxfId="191" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{64EEA08C-5481-4401-BC85-B2556C39EB6B}" name="QP" totalsRowFunction="sum" totalsRowDxfId="202" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S2.2[[#This Row],[CU]]*S2.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5534,20 +5791,20 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3A55ED19-6706-4542-8537-8BBE47EA7476}" name="S3.1" displayName="S3.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="190" dataDxfId="189" totalsRowDxfId="188">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{3A55ED19-6706-4542-8537-8BBE47EA7476}" name="S3.1" displayName="S3.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="201" dataDxfId="200" totalsRowDxfId="199">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{D18EF69B-4B91-43C6-84DA-7E2A52C7B3E7}" name="Course Code" totalsRowLabel="Total" dataDxfId="187" totalsRowDxfId="186"/>
-    <tableColumn id="2" xr3:uid="{87C4A3FF-BC48-4384-A6E2-63149B5E7575}" name="Course Title" dataDxfId="185" totalsRowDxfId="184"/>
-    <tableColumn id="3" xr3:uid="{90989901-F6C9-47BC-930A-B649A0C25513}" name="CU" totalsRowFunction="sum" totalsRowDxfId="183" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{A88EDD5C-01A4-40E6-A784-A342F5F35E66}" name="Mark" totalsRowDxfId="182" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{44F6407C-CFDA-4AF6-9CDA-9548F5A9223B}" name="Grade" totalsRowDxfId="181" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{D18EF69B-4B91-43C6-84DA-7E2A52C7B3E7}" name="Course Code" totalsRowLabel="Total" dataDxfId="198" totalsRowDxfId="197"/>
+    <tableColumn id="2" xr3:uid="{87C4A3FF-BC48-4384-A6E2-63149B5E7575}" name="Course Title" dataDxfId="196" totalsRowDxfId="195"/>
+    <tableColumn id="3" xr3:uid="{90989901-F6C9-47BC-930A-B649A0C25513}" name="CU" totalsRowFunction="sum" totalsRowDxfId="194" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{A88EDD5C-01A4-40E6-A784-A342F5F35E66}" name="Mark" totalsRowDxfId="193" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{44F6407C-CFDA-4AF6-9CDA-9548F5A9223B}" name="Grade" totalsRowDxfId="192" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S3.1[[#This Row],[Mark]]="","",IF(AND(LEN(S3.1[[#This Row],[Course Code]])=10, S3.1[[#This Row],[Mark]]&gt;=60),"C",IF(S3.1[[#This Row],[Mark]]&lt;40,"F",IF(S3.1[[#This Row],[Mark]]&lt;45,"E",IF(S3.1[[#This Row],[Mark]]&lt;50,"D",IF(S3.1[[#This Row],[Mark]]&lt;60,"C",IF(S3.1[[#This Row],[Mark]]&lt;70,"B",IF(S3.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{E73FF6F6-229C-4669-AC2D-FAF982A7129D}" name="GP" totalsRowDxfId="180" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{E73FF6F6-229C-4669-AC2D-FAF982A7129D}" name="GP" totalsRowDxfId="191" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S3.1[[#This Row],[Mark]]="","",IF(AND(LEN(S3.1[[#This Row],[Course Code]])=10, S3.1[[#This Row],[Mark]]&gt;=60),3,IF(S3.1[[#This Row],[Mark]]&lt;40,0,IF(S3.1[[#This Row],[Mark]]&lt;45,1,IF(S3.1[[#This Row],[Mark]]&lt;50,2,IF(S3.1[[#This Row],[Mark]]&lt;60,3,IF(S3.1[[#This Row],[Mark]]&lt;70,4,IF(S3.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{97CA79E0-1675-44FE-95F8-CA7944417F59}" name="QP" totalsRowFunction="sum" totalsRowDxfId="179" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{97CA79E0-1675-44FE-95F8-CA7944417F59}" name="QP" totalsRowFunction="sum" totalsRowDxfId="190" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S3.1[[#This Row],[CU]]*S3.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5556,20 +5813,20 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0EE398F5-1FE4-437C-8F02-EB87731559DF}" name="S3.2" displayName="S3.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="178" dataDxfId="177" totalsRowDxfId="176">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{0EE398F5-1FE4-437C-8F02-EB87731559DF}" name="S3.2" displayName="S3.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="189" dataDxfId="188" totalsRowDxfId="187">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{B195FD40-6FF3-426F-BF52-3639DD800F63}" name="Course Code" totalsRowLabel="Total" dataDxfId="175" totalsRowDxfId="174"/>
-    <tableColumn id="2" xr3:uid="{CEF49805-4990-425E-9138-861368275F69}" name="Course Title" dataDxfId="173" totalsRowDxfId="172"/>
-    <tableColumn id="3" xr3:uid="{020837AE-2E78-4377-8A08-D56637C65392}" name="CU" totalsRowFunction="sum" totalsRowDxfId="171" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{574F6558-76DC-4F6A-AE0A-02B3A01D5153}" name="Mark" totalsRowDxfId="170" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{00CC7CE1-C72F-44E9-8AD1-FD07D5594CE8}" name="Grade" totalsRowDxfId="169" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{B195FD40-6FF3-426F-BF52-3639DD800F63}" name="Course Code" totalsRowLabel="Total" dataDxfId="186" totalsRowDxfId="185"/>
+    <tableColumn id="2" xr3:uid="{CEF49805-4990-425E-9138-861368275F69}" name="Course Title" dataDxfId="184" totalsRowDxfId="183"/>
+    <tableColumn id="3" xr3:uid="{020837AE-2E78-4377-8A08-D56637C65392}" name="CU" totalsRowFunction="sum" totalsRowDxfId="182" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{574F6558-76DC-4F6A-AE0A-02B3A01D5153}" name="Mark" totalsRowDxfId="181" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{00CC7CE1-C72F-44E9-8AD1-FD07D5594CE8}" name="Grade" totalsRowDxfId="180" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S3.2[[#This Row],[Mark]]="","",IF(AND(LEN(S3.2[[#This Row],[Course Code]])=10, S3.2[[#This Row],[Mark]]&gt;=60),"C",IF(S3.2[[#This Row],[Mark]]&lt;40,"F",IF(S3.2[[#This Row],[Mark]]&lt;45,"E",IF(S3.2[[#This Row],[Mark]]&lt;50,"D",IF(S3.2[[#This Row],[Mark]]&lt;60,"C",IF(S3.2[[#This Row],[Mark]]&lt;70,"B",IF(S3.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{F6298398-80B0-4F72-833E-D0A7B334B3A0}" name="GP" totalsRowDxfId="168" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{F6298398-80B0-4F72-833E-D0A7B334B3A0}" name="GP" totalsRowDxfId="179" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S3.2[[#This Row],[Mark]]="","",IF(AND(LEN(S3.2[[#This Row],[Course Code]])=10, S3.2[[#This Row],[Mark]]&gt;=60),3,IF(S3.2[[#This Row],[Mark]]&lt;40,0,IF(S3.2[[#This Row],[Mark]]&lt;45,1,IF(S3.2[[#This Row],[Mark]]&lt;50,2,IF(S3.2[[#This Row],[Mark]]&lt;60,3,IF(S3.2[[#This Row],[Mark]]&lt;70,4,IF(S3.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{DC3DE242-81C1-4798-BAAA-1AA23F9F57A9}" name="QP" totalsRowFunction="sum" totalsRowDxfId="167" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{DC3DE242-81C1-4798-BAAA-1AA23F9F57A9}" name="QP" totalsRowFunction="sum" totalsRowDxfId="178" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S3.2[[#This Row],[CU]]*S3.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5578,20 +5835,20 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9D20ED8C-7D8D-4810-A2F7-6110E6EE0CBF}" name="S4.1" displayName="S4.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="166" dataDxfId="165" totalsRowDxfId="164">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{9D20ED8C-7D8D-4810-A2F7-6110E6EE0CBF}" name="S4.1" displayName="S4.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="177" dataDxfId="176" totalsRowDxfId="175">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{1D04466F-90FB-4E91-BB8B-332EE3FF37F7}" name="Course Code" totalsRowLabel="Total" dataDxfId="163" totalsRowDxfId="162"/>
-    <tableColumn id="2" xr3:uid="{C2DFB37D-6A23-408E-874D-CFDD15B0F192}" name="Course Title" dataDxfId="161" totalsRowDxfId="160"/>
-    <tableColumn id="3" xr3:uid="{28A51089-2E4D-4C1E-A1FF-01ABCF11383E}" name="CU" totalsRowFunction="sum" totalsRowDxfId="159" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{D48867A4-BE47-4CBD-BD6B-49ACA4AAAE6D}" name="Mark" totalsRowDxfId="158" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{B750E9ED-73AB-4C12-B221-67056BBD68C2}" name="Grade" totalsRowDxfId="157" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{1D04466F-90FB-4E91-BB8B-332EE3FF37F7}" name="Course Code" totalsRowLabel="Total" dataDxfId="174" totalsRowDxfId="173"/>
+    <tableColumn id="2" xr3:uid="{C2DFB37D-6A23-408E-874D-CFDD15B0F192}" name="Course Title" dataDxfId="172" totalsRowDxfId="171"/>
+    <tableColumn id="3" xr3:uid="{28A51089-2E4D-4C1E-A1FF-01ABCF11383E}" name="CU" totalsRowFunction="sum" totalsRowDxfId="170" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{D48867A4-BE47-4CBD-BD6B-49ACA4AAAE6D}" name="Mark" totalsRowDxfId="169" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{B750E9ED-73AB-4C12-B221-67056BBD68C2}" name="Grade" totalsRowDxfId="168" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S4.1[[#This Row],[Mark]]="","",IF(AND(LEN(S4.1[[#This Row],[Course Code]])=10, S4.1[[#This Row],[Mark]]&gt;=60),"C",IF(S4.1[[#This Row],[Mark]]&lt;40,"F",IF(S4.1[[#This Row],[Mark]]&lt;45,"E",IF(S4.1[[#This Row],[Mark]]&lt;50,"D",IF(S4.1[[#This Row],[Mark]]&lt;60,"C",IF(S4.1[[#This Row],[Mark]]&lt;70,"B",IF(S4.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{8DA6BBB8-FAD1-42AB-9F71-6A33875AC2D5}" name="GP" totalsRowDxfId="156" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{8DA6BBB8-FAD1-42AB-9F71-6A33875AC2D5}" name="GP" totalsRowDxfId="167" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S4.1[[#This Row],[Mark]]="","",IF(AND(LEN(S4.1[[#This Row],[Course Code]])=10, S4.1[[#This Row],[Mark]]&gt;=60),3,IF(S4.1[[#This Row],[Mark]]&lt;40,0,IF(S4.1[[#This Row],[Mark]]&lt;45,1,IF(S4.1[[#This Row],[Mark]]&lt;50,2,IF(S4.1[[#This Row],[Mark]]&lt;60,3,IF(S4.1[[#This Row],[Mark]]&lt;70,4,IF(S4.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A5C049D7-F102-4C73-98DF-DC6C9E590523}" name="QP" totalsRowFunction="sum" totalsRowDxfId="155" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{A5C049D7-F102-4C73-98DF-DC6C9E590523}" name="QP" totalsRowFunction="sum" totalsRowDxfId="166" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S4.1[[#This Row],[CU]]*S4.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5600,20 +5857,20 @@
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{30DC811C-80CD-4F69-AFDB-144BD0BCA6D8}" name="S4.2" displayName="S4.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="154" dataDxfId="153" totalsRowDxfId="152">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{30DC811C-80CD-4F69-AFDB-144BD0BCA6D8}" name="S4.2" displayName="S4.2" ref="A15:G17" totalsRowCount="1" headerRowDxfId="165" dataDxfId="164" totalsRowDxfId="163">
   <autoFilter ref="A15:G16" xr:uid="{72C67E04-0524-4B66-B663-358AE858E0AF}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{A4297557-CA6A-4794-94DB-61ACCAAAF5B3}" name="Course Code" totalsRowLabel="Total" dataDxfId="151" totalsRowDxfId="150"/>
-    <tableColumn id="2" xr3:uid="{EC77BE9A-1B0B-4966-B219-7D35BA4B75C7}" name="Course Title" dataDxfId="149" totalsRowDxfId="148"/>
-    <tableColumn id="3" xr3:uid="{AF25DB81-E40A-4D38-8EE0-E2BC6DC2FC5A}" name="CU" totalsRowFunction="sum" totalsRowDxfId="147" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{6EB53A13-FF89-4F49-9DAF-4A48D3A39828}" name="Mark" totalsRowDxfId="146" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{F5C230B0-3AFA-42CE-9F15-81CDA9E071EE}" name="Grade" totalsRowDxfId="145" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{A4297557-CA6A-4794-94DB-61ACCAAAF5B3}" name="Course Code" totalsRowLabel="Total" dataDxfId="162" totalsRowDxfId="161"/>
+    <tableColumn id="2" xr3:uid="{EC77BE9A-1B0B-4966-B219-7D35BA4B75C7}" name="Course Title" dataDxfId="160" totalsRowDxfId="159"/>
+    <tableColumn id="3" xr3:uid="{AF25DB81-E40A-4D38-8EE0-E2BC6DC2FC5A}" name="CU" totalsRowFunction="sum" totalsRowDxfId="158" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{6EB53A13-FF89-4F49-9DAF-4A48D3A39828}" name="Mark" totalsRowDxfId="157" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{F5C230B0-3AFA-42CE-9F15-81CDA9E071EE}" name="Grade" totalsRowDxfId="156" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S4.2[[#This Row],[Mark]]="","",IF(AND(LEN(S4.2[[#This Row],[Course Code]])=10, S4.2[[#This Row],[Mark]]&gt;=60),"C",IF(S4.2[[#This Row],[Mark]]&lt;40,"F",IF(S4.2[[#This Row],[Mark]]&lt;45,"E",IF(S4.2[[#This Row],[Mark]]&lt;50,"D",IF(S4.2[[#This Row],[Mark]]&lt;60,"C",IF(S4.2[[#This Row],[Mark]]&lt;70,"B",IF(S4.2[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{418992FB-EEF5-4874-A92C-5BA5ED94E7FC}" name="GP" totalsRowDxfId="144" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{418992FB-EEF5-4874-A92C-5BA5ED94E7FC}" name="GP" totalsRowDxfId="155" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S4.2[[#This Row],[Mark]]="","",IF(AND(LEN(S4.2[[#This Row],[Course Code]])=10, S4.2[[#This Row],[Mark]]&gt;=60),3,IF(S4.2[[#This Row],[Mark]]&lt;40,0,IF(S4.2[[#This Row],[Mark]]&lt;45,1,IF(S4.2[[#This Row],[Mark]]&lt;50,2,IF(S4.2[[#This Row],[Mark]]&lt;60,3,IF(S4.2[[#This Row],[Mark]]&lt;70,4,IF(S4.2[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{D6B978F9-705C-443E-846F-EAA2C269EB6B}" name="QP" totalsRowFunction="sum" totalsRowDxfId="143" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{D6B978F9-705C-443E-846F-EAA2C269EB6B}" name="QP" totalsRowFunction="sum" totalsRowDxfId="154" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S4.2[[#This Row],[CU]]*S4.2[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5622,20 +5879,20 @@
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1599AB26-9407-4A14-A9F5-9292DA6A95F0}" name="S5.1" displayName="S5.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="142" dataDxfId="141" totalsRowDxfId="140">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{1599AB26-9407-4A14-A9F5-9292DA6A95F0}" name="S5.1" displayName="S5.1" ref="A10:G12" totalsRowCount="1" headerRowDxfId="153" dataDxfId="152" totalsRowDxfId="151">
   <autoFilter ref="A10:G11" xr:uid="{2166DBE8-2D77-4679-B3C1-17AB4323FA7C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{336B08B4-F01F-4BBC-A43A-1B56D6B7693C}" name="Course Code" totalsRowLabel="Total" dataDxfId="139" totalsRowDxfId="138"/>
-    <tableColumn id="2" xr3:uid="{52D04E96-856A-4A0B-B556-B17C071B6569}" name="Course Title" dataDxfId="137" totalsRowDxfId="136"/>
-    <tableColumn id="3" xr3:uid="{7CF22717-A719-49E8-8010-18C3F58FDC39}" name="CU" totalsRowFunction="sum" totalsRowDxfId="135" dataCellStyle="Number Style"/>
-    <tableColumn id="4" xr3:uid="{E5F42800-6FBC-4D11-885C-42E6362F1499}" name="Mark" totalsRowDxfId="134" dataCellStyle="Number Style"/>
-    <tableColumn id="5" xr3:uid="{8DFB5FB2-C3FB-4948-89D8-57E8850F3E7E}" name="Grade" totalsRowDxfId="133" dataCellStyle="Number Style">
+    <tableColumn id="1" xr3:uid="{336B08B4-F01F-4BBC-A43A-1B56D6B7693C}" name="Course Code" totalsRowLabel="Total" dataDxfId="150" totalsRowDxfId="149"/>
+    <tableColumn id="2" xr3:uid="{52D04E96-856A-4A0B-B556-B17C071B6569}" name="Course Title" dataDxfId="148" totalsRowDxfId="147"/>
+    <tableColumn id="3" xr3:uid="{7CF22717-A719-49E8-8010-18C3F58FDC39}" name="CU" totalsRowFunction="sum" totalsRowDxfId="146" dataCellStyle="Number Style"/>
+    <tableColumn id="4" xr3:uid="{E5F42800-6FBC-4D11-885C-42E6362F1499}" name="Mark" totalsRowDxfId="145" dataCellStyle="Number Style"/>
+    <tableColumn id="5" xr3:uid="{8DFB5FB2-C3FB-4948-89D8-57E8850F3E7E}" name="Grade" totalsRowDxfId="144" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S5.1[[#This Row],[Mark]]="","",IF(AND(LEN(S5.1[[#This Row],[Course Code]])=10, S5.1[[#This Row],[Mark]]&gt;=60),"C",IF(S5.1[[#This Row],[Mark]]&lt;40,"F",IF(S5.1[[#This Row],[Mark]]&lt;45,"E",IF(S5.1[[#This Row],[Mark]]&lt;50,"D",IF(S5.1[[#This Row],[Mark]]&lt;60,"C",IF(S5.1[[#This Row],[Mark]]&lt;70,"B",IF(S5.1[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{001241F0-D717-45BB-84C0-6E619433CF05}" name="GP" totalsRowDxfId="132" dataCellStyle="Number Style">
+    <tableColumn id="6" xr3:uid="{001241F0-D717-45BB-84C0-6E619433CF05}" name="GP" totalsRowDxfId="143" dataCellStyle="Number Style">
       <calculatedColumnFormula>IF(S5.1[[#This Row],[Mark]]="","",IF(AND(LEN(S5.1[[#This Row],[Course Code]])=10, S5.1[[#This Row],[Mark]]&gt;=60),3,IF(S5.1[[#This Row],[Mark]]&lt;40,0,IF(S5.1[[#This Row],[Mark]]&lt;45,1,IF(S5.1[[#This Row],[Mark]]&lt;50,2,IF(S5.1[[#This Row],[Mark]]&lt;60,3,IF(S5.1[[#This Row],[Mark]]&lt;70,4,IF(S5.1[[#This Row],[Mark]]&lt;=100,5, ""))))))))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{A89F0EB7-A761-45C9-AB60-D278A5AF51F1}" name="QP" totalsRowFunction="sum" totalsRowDxfId="131" dataCellStyle="Number Style">
+    <tableColumn id="7" xr3:uid="{A89F0EB7-A761-45C9-AB60-D278A5AF51F1}" name="QP" totalsRowFunction="sum" totalsRowDxfId="142" dataCellStyle="Number Style">
       <calculatedColumnFormula>IFERROR(S5.1[[#This Row],[CU]]*S5.1[[#This Row],[GP]], "")</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -5958,48 +6215,48 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="63" t="s">
+      <c r="A1" s="65" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="65"/>
+      <c r="G1" s="65"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
-      <c r="G2" s="64"/>
+      <c r="B2" s="66"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="64"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="64"/>
-      <c r="F3" s="64"/>
-      <c r="G3" s="64"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
+      <c r="E3" s="66"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="61" t="s">
+      <c r="A4" s="63" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="61"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="61"/>
-      <c r="F4" s="61"/>
-      <c r="G4" s="61"/>
+      <c r="B4" s="63"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="9"/>
@@ -6018,20 +6275,20 @@
       <c r="C6" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="65"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="65"/>
-      <c r="G6" s="66"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="68"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="44" t="s">
         <v>17</v>
       </c>
       <c r="B7" s="12"/>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="60"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="12"/>
       <c r="F7" s="13" t="s">
         <v>15</v>
@@ -6039,15 +6296,15 @@
       <c r="G7" s="14"/>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="61" t="s">
+      <c r="A9" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="61"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="8" t="s">
@@ -6260,7 +6517,7 @@
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.6171875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.1875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="8" customWidth="1"/>
     <col min="3" max="5" width="7.5234375" style="8" customWidth="1"/>
     <col min="6" max="6" width="13.80859375" style="8" customWidth="1"/>
     <col min="7" max="7" width="102.94921875" style="8" customWidth="1"/>
@@ -6268,49 +6525,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="G1" s="58"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="58"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="58"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="65" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
       <c r="G6" s="58"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
@@ -6520,56 +6777,56 @@
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="13.6171875" style="8" customWidth="1"/>
-    <col min="2" max="2" width="33.1875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="8" customWidth="1"/>
     <col min="3" max="5" width="7.5234375" style="8" customWidth="1"/>
     <col min="6" max="6" width="13.80859375" style="8" customWidth="1"/>
     <col min="7" max="16384" width="8.6640625" style="8"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="G1" s="53"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
       <c r="G2" s="53"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
       <c r="G3" s="53"/>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="63" t="s">
+      <c r="A6" s="65" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="63"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A7"/>
@@ -6632,6 +6889,259 @@
       </c>
       <c r="C12" s="34">
         <f>SUBTOTAL(109,Unknown[CU])</f>
+        <v>0</v>
+      </c>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+    </row>
+    <row r="14" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A17"/>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A18"/>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A19"/>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+    <row r="20" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A20"/>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+    </row>
+    <row r="21" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A21"/>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+    </row>
+    <row r="22" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A22"/>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+    </row>
+    <row r="23" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A23"/>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A24"/>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+    </row>
+    <row r="25" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A25"/>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+    </row>
+    <row r="26" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A26"/>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+    </row>
+  </sheetData>
+  <sheetProtection selectLockedCells="1"/>
+  <mergeCells count="4">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:F2"/>
+    <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A6:F6"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup fitToHeight="0" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <tableParts count="1">
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB83EB46-8BBA-4A23-9A05-FC127F36547A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:G26"/>
+  <sheetViews>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="13.6171875" style="8" customWidth="1"/>
+    <col min="2" max="2" width="43.76171875" style="8" customWidth="1"/>
+    <col min="3" max="5" width="7.5234375" style="8" customWidth="1"/>
+    <col min="6" max="6" width="13.80859375" style="8" customWidth="1"/>
+    <col min="7" max="16384" width="8.6640625" style="8"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="70" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="53"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A2" s="70" t="str">
+        <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
+        <v>Faculty</v>
+      </c>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="53"/>
+    </row>
+    <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A3" s="70" t="str">
+        <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
+        <v>Department</v>
+      </c>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="53"/>
+    </row>
+    <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A6" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="65"/>
+      <c r="C6" s="65"/>
+      <c r="D6" s="65"/>
+      <c r="E6" s="65"/>
+      <c r="F6" s="65"/>
+    </row>
+    <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
+      <c r="A9" s="60"/>
+      <c r="B9" s="60"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="61"/>
+      <c r="E9" s="61"/>
+      <c r="F9" s="61"/>
+    </row>
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A11" s="15"/>
+      <c r="B11" s="15"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38" t="str">
+        <f>IF(Outstanding[[#This Row],[Mark]]="","",IF(AND(LEN(Outstanding[[#This Row],[Course Code]])=10, Outstanding[[#This Row],[Mark]]&gt;=60),"C",IF(Outstanding[[#This Row],[Mark]]&lt;40,"F",IF(Outstanding[[#This Row],[Mark]]&lt;45,"E",IF(Outstanding[[#This Row],[Mark]]&lt;50,"D",IF(Outstanding[[#This Row],[Mark]]&lt;60,"C",IF(Outstanding[[#This Row],[Mark]]&lt;70,"B",IF(Outstanding[[#This Row],[Mark]]&lt;=100,"A", ""))))))))</f>
+        <v/>
+      </c>
+      <c r="F11" s="38"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A12" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C12" s="34">
+        <f>SUBTOTAL(109,Outstanding[CU])</f>
         <v>0</v>
       </c>
       <c r="D12" s="34"/>
@@ -6779,50 +7289,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
@@ -6844,13 +7354,13 @@
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -6860,10 +7370,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -6877,15 +7387,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -7107,50 +7617,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
@@ -7172,13 +7682,13 @@
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -7188,10 +7698,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -7205,15 +7715,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -7435,50 +7945,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
@@ -7500,13 +8010,13 @@
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -7516,10 +8026,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -7533,15 +8043,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -7793,50 +8303,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
@@ -7858,13 +8368,13 @@
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -7874,10 +8384,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -7891,15 +8401,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -8154,50 +8664,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
@@ -8219,13 +8729,13 @@
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -8235,10 +8745,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -8252,15 +8762,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -8516,50 +9026,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="21"/>
@@ -8581,13 +9091,13 @@
       <c r="C6" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -8597,10 +9107,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="23" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -8614,15 +9124,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -8878,50 +9388,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="48"/>
@@ -8943,13 +9453,13 @@
       <c r="C6" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -8959,10 +9469,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="50" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -8976,15 +9486,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">
@@ -9240,50 +9750,50 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="70" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
+      <c r="G1" s="70"/>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="68" t="str">
+      <c r="A2" s="70" t="str">
         <f>IF('L100'!A2:G2="","",'L100'!A2:G2)</f>
         <v>Faculty</v>
       </c>
-      <c r="B2" s="68"/>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="68"/>
-      <c r="F2" s="68"/>
-      <c r="G2" s="68"/>
+      <c r="B2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
     </row>
     <row r="3" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="70" t="str">
         <f>IF('L100'!A3:G3="","",'L100'!A3:G3)</f>
         <v>Department</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="68"/>
+      <c r="B3" s="70"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="70"/>
+      <c r="G3" s="70"/>
     </row>
     <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A4" s="67" t="s">
+      <c r="A4" s="69" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="67"/>
-      <c r="C4" s="67"/>
-      <c r="D4" s="67"/>
-      <c r="E4" s="67"/>
-      <c r="F4" s="67"/>
-      <c r="G4" s="67"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="69"/>
+      <c r="E4" s="69"/>
+      <c r="F4" s="69"/>
+      <c r="G4" s="69"/>
     </row>
     <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A5" s="48"/>
@@ -9305,13 +9815,13 @@
       <c r="C6" s="49" t="s">
         <v>18</v>
       </c>
-      <c r="D6" s="69" t="str">
+      <c r="D6" s="71" t="str">
         <f>IF('L100'!D6:G6="","",'L100'!D6:G6)</f>
         <v/>
       </c>
-      <c r="E6" s="69"/>
-      <c r="F6" s="69"/>
-      <c r="G6" s="70"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="72"/>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A7" s="40" t="s">
@@ -9321,10 +9831,10 @@
         <f>IF('L100'!B7="","",'L100'!B7)</f>
         <v/>
       </c>
-      <c r="C7" s="71" t="s">
+      <c r="C7" s="73" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="71"/>
+      <c r="D7" s="73"/>
       <c r="E7" s="50" t="str">
         <f>IF('L100'!E7="","",'L100'!E7)</f>
         <v/>
@@ -9338,15 +9848,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A9" s="67" t="s">
+      <c r="A9" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B9" s="67"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="62"/>
-      <c r="G9" s="62"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
     </row>
     <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A10" s="20" t="s">

</xml_diff>